<commit_message>
Setting up the data importer
</commit_message>
<xml_diff>
--- a/UntitledKitchenGame/Game/UntitledKitchenGame/Assets/Editor/Items.xlsx
+++ b/UntitledKitchenGame/Game/UntitledKitchenGame/Assets/Editor/Items.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\murra\OneDrive\Documents\GitHub\UntitledKitchenGame\UntitledKitchenGame\Game\UntitledKitchenGame\Assets\Editor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6D6AFB4D-F285-4EAD-BC7D-7CF8B4DB7FE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFBF26F8-97AF-49E0-8A7D-B81DFB1C254A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F8B15126-9F65-4AA0-BFBE-7FC0EBE8032D}"/>
   </bookViews>
@@ -41,9 +41,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
-    <t>Food</t>
-  </si>
-  <si>
     <t>Points</t>
   </si>
   <si>
@@ -78,6 +75,9 @@
   </si>
   <si>
     <t>Bread</t>
+  </si>
+  <si>
+    <t>Name</t>
   </si>
 </sst>
 </file>
@@ -113,12 +113,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,7 +471,7 @@
   <dimension ref="B3:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -483,102 +482,102 @@
   <sheetData>
     <row r="3" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="F3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D4">
         <v>10</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4">
         <v>100</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D5">
         <v>10</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5">
         <v>100</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D6">
         <v>10</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6">
         <v>100</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="H6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7">
         <v>10</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7">
         <v>100</v>
       </c>
       <c r="F7">
         <v>1</v>
       </c>
       <c r="H7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -603,6 +602,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="97dd5345-e793-494f-a61a-0ff5f2d8588d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EB9F34A24037AB4FA470085E68A4B53B" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1f05ce8c82e9282909648c3323760eae">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="97dd5345-e793-494f-a61a-0ff5f2d8588d" xmlns:ns4="72e2bb9d-dac6-4618-b85f-5ec835598a0c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c14bf05b446930f087596548c801372f" ns3:_="" ns4:_="">
     <xsd:import namespace="97dd5345-e793-494f-a61a-0ff5f2d8588d"/>
@@ -829,24 +845,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="97dd5345-e793-494f-a61a-0ff5f2d8588d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA6B1F78-6D1D-4550-867C-D81A2584596E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="72e2bb9d-dac6-4618-b85f-5ec835598a0c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="97dd5345-e793-494f-a61a-0ff5f2d8588d"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB2BC082-80AE-42F8-9667-95CF6F1F5700}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{65537B17-CCB8-447E-A12B-556BEEDE4DB0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -863,29 +887,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB2BC082-80AE-42F8-9667-95CF6F1F5700}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA6B1F78-6D1D-4550-867C-D81A2584596E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="72e2bb9d-dac6-4618-b85f-5ec835598a0c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="97dd5345-e793-494f-a61a-0ff5f2d8588d"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Food items are now generated with the excel table
Now working on how the order system might work
</commit_message>
<xml_diff>
--- a/UntitledKitchenGame/Game/UntitledKitchenGame/Assets/Editor/Items.xlsx
+++ b/UntitledKitchenGame/Game/UntitledKitchenGame/Assets/Editor/Items.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\murra\OneDrive\Documents\GitHub\UntitledKitchenGame\UntitledKitchenGame\Game\UntitledKitchenGame\Assets\Editor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFBF26F8-97AF-49E0-8A7D-B81DFB1C254A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FF9CBDF-AE55-45ED-9110-161E022AD6CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F8B15126-9F65-4AA0-BFBE-7FC0EBE8032D}"/>
   </bookViews>
@@ -38,8 +38,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>Points</t>
   </si>
@@ -78,6 +100,18 @@
   </si>
   <si>
     <t>Name</t>
+  </si>
+  <si>
+    <t>Order</t>
+  </si>
+  <si>
+    <t>Item 1</t>
+  </si>
+  <si>
+    <t>Item 2</t>
+  </si>
+  <si>
+    <t>Item 3</t>
   </si>
 </sst>
 </file>
@@ -122,7 +156,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -140,7 +177,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{35FB6A7E-F941-41ED-AF7A-CE78317F833A}" name="ItemTypes" displayName="ItemTypes" ref="H3:H7" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{35FB6A7E-F941-41ED-AF7A-CE78317F833A}" name="ItemTypes" displayName="ItemTypes" ref="H3:H7" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="H3:H7" xr:uid="{35FB6A7E-F941-41ED-AF7A-CE78317F833A}">
     <filterColumn colId="0" hiddenButton="1"/>
   </autoFilter>
@@ -148,6 +185,26 @@
     <tableColumn id="1" xr3:uid="{5DF97B08-7333-43C7-AFD3-4654928C6ED9}" name="Type"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7AE9A713-C3CE-48AC-B440-488A7CD3381A}" name="Food" displayName="Food" ref="B3:F7" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="B3:F7" xr:uid="{7AE9A713-C3CE-48AC-B440-488A7CD3381A}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{680C3E85-364D-401E-80B1-7407A04F49D6}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{0D89CADA-83AE-47AD-A23D-3024EF536ED5}" name="Type"/>
+    <tableColumn id="3" xr3:uid="{0E390CF0-6660-4FA1-802C-60388EBB3793}" name="Points"/>
+    <tableColumn id="4" xr3:uid="{114CD449-19F8-4A9E-A244-663C39E5FA57}" name="Rarity"/>
+    <tableColumn id="5" xr3:uid="{C880951D-D59D-4C6D-B41D-38AACAC34851}" name="Stages"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -468,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2334730F-D581-4249-91BD-F969B819BCBB}">
-  <dimension ref="B3:H7"/>
+  <dimension ref="B3:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,7 +537,7 @@
     <col min="8" max="8" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
@@ -499,8 +556,20 @@
       <c r="H3" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="J3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>7</v>
       </c>
@@ -519,8 +588,20 @@
       <c r="H4" t="s">
         <v>4</v>
       </c>
+      <c r="K4" t="str" cm="1">
+        <f t="array" aca="1" ref="K4" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
+        <v>Bread</v>
+      </c>
+      <c r="L4" t="str" cm="1">
+        <f t="array" aca="1" ref="L4" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
+        <v>Beef</v>
+      </c>
+      <c r="M4" t="str" cm="1">
+        <f t="array" aca="1" ref="M4" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
+        <v>Bread</v>
+      </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>8</v>
       </c>
@@ -539,8 +620,20 @@
       <c r="H5" t="s">
         <v>5</v>
       </c>
+      <c r="K5" t="str" cm="1">
+        <f t="array" aca="1" ref="K5" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
+        <v>Beef</v>
+      </c>
+      <c r="L5" t="str" cm="1">
+        <f t="array" aca="1" ref="L5" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
+        <v>Carrot</v>
+      </c>
+      <c r="M5" t="str" cm="1">
+        <f t="array" aca="1" ref="M5" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
+        <v>Bread</v>
+      </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>9</v>
       </c>
@@ -559,8 +652,20 @@
       <c r="H6" t="s">
         <v>6</v>
       </c>
+      <c r="K6" t="str" cm="1">
+        <f t="array" aca="1" ref="K6" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
+        <v>Beef</v>
+      </c>
+      <c r="L6" t="str" cm="1">
+        <f t="array" aca="1" ref="L6" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
+        <v>Carrot</v>
+      </c>
+      <c r="M6" t="str" cm="1">
+        <f t="array" aca="1" ref="M6" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
+        <v>Beef</v>
+      </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>11</v>
       </c>
@@ -578,6 +683,18 @@
       </c>
       <c r="H7" t="s">
         <v>10</v>
+      </c>
+      <c r="K7" t="str" cm="1">
+        <f t="array" aca="1" ref="K7" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
+        <v>Salmon</v>
+      </c>
+      <c r="L7" t="str" cm="1">
+        <f t="array" aca="1" ref="L7" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
+        <v>Beef</v>
+      </c>
+      <c r="M7" t="str" cm="1">
+        <f t="array" aca="1" ref="M7" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
+        <v>Bread</v>
       </c>
     </row>
   </sheetData>
@@ -595,8 +712,9 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Added more food items
</commit_message>
<xml_diff>
--- a/UntitledKitchenGame/Game/UntitledKitchenGame/Assets/Editor/Items.xlsx
+++ b/UntitledKitchenGame/Game/UntitledKitchenGame/Assets/Editor/Items.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\murra\OneDrive\Documents\GitHub\UntitledKitchenGame\UntitledKitchenGame\Game\UntitledKitchenGame\Assets\Editor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FF9CBDF-AE55-45ED-9110-161E022AD6CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04441F26-4237-42E1-A3B1-7216193CCF77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F8B15126-9F65-4AA0-BFBE-7FC0EBE8032D}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F8B15126-9F65-4AA0-BFBE-7FC0EBE8032D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
   <si>
     <t>Points</t>
   </si>
@@ -112,6 +112,30 @@
   </si>
   <si>
     <t>Item 3</t>
+  </si>
+  <si>
+    <t>Pork</t>
+  </si>
+  <si>
+    <t>Chicken</t>
+  </si>
+  <si>
+    <t>Tuna</t>
+  </si>
+  <si>
+    <t>Lobster</t>
+  </si>
+  <si>
+    <t>Pasta</t>
+  </si>
+  <si>
+    <t>Rice</t>
+  </si>
+  <si>
+    <t>Onion</t>
+  </si>
+  <si>
+    <t>Lettuce</t>
   </si>
 </sst>
 </file>
@@ -189,14 +213,11 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7AE9A713-C3CE-48AC-B440-488A7CD3381A}" name="Food" displayName="Food" ref="B3:F7" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="B3:F7" xr:uid="{7AE9A713-C3CE-48AC-B440-488A7CD3381A}">
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-    <filterColumn colId="2" hiddenButton="1"/>
-    <filterColumn colId="3" hiddenButton="1"/>
-    <filterColumn colId="4" hiddenButton="1"/>
-  </autoFilter>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7AE9A713-C3CE-48AC-B440-488A7CD3381A}" name="Food" displayName="Food" ref="B3:F15" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="B3:F15" xr:uid="{7AE9A713-C3CE-48AC-B440-488A7CD3381A}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:F15">
+    <sortCondition ref="C3:C15"/>
+  </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{680C3E85-364D-401E-80B1-7407A04F49D6}" name="Name"/>
     <tableColumn id="2" xr3:uid="{0D89CADA-83AE-47AD-A23D-3024EF536ED5}" name="Type"/>
@@ -525,10 +546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2334730F-D581-4249-91BD-F969B819BCBB}">
-  <dimension ref="B3:M7"/>
+  <dimension ref="B3:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S7" sqref="S7"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,10 +592,10 @@
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D4">
         <v>10</v>
@@ -590,11 +611,11 @@
       </c>
       <c r="K4" t="str" cm="1">
         <f t="array" aca="1" ref="K4" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Bread</v>
+        <v>Beef</v>
       </c>
       <c r="L4" t="str" cm="1">
         <f t="array" aca="1" ref="L4" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Beef</v>
+        <v>Lobster</v>
       </c>
       <c r="M4" t="str" cm="1">
         <f t="array" aca="1" ref="M4" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
@@ -603,10 +624,10 @@
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D5">
         <v>10</v>
@@ -622,20 +643,20 @@
       </c>
       <c r="K5" t="str" cm="1">
         <f t="array" aca="1" ref="K5" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Beef</v>
+        <v>Rice</v>
       </c>
       <c r="L5" t="str" cm="1">
         <f t="array" aca="1" ref="L5" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Carrot</v>
+        <v>Pork</v>
       </c>
       <c r="M5" t="str" cm="1">
         <f t="array" aca="1" ref="M5" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Bread</v>
+        <v>Beef</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -654,15 +675,15 @@
       </c>
       <c r="K6" t="str" cm="1">
         <f t="array" aca="1" ref="K6" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Beef</v>
+        <v>Tuna</v>
       </c>
       <c r="L6" t="str" cm="1">
         <f t="array" aca="1" ref="L6" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Carrot</v>
+        <v>Rice</v>
       </c>
       <c r="M6" t="str" cm="1">
         <f t="array" aca="1" ref="M6" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Beef</v>
+        <v>Tuna</v>
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
@@ -686,27 +707,163 @@
       </c>
       <c r="K7" t="str" cm="1">
         <f t="array" aca="1" ref="K7" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Salmon</v>
+        <v>Rice</v>
       </c>
       <c r="L7" t="str" cm="1">
         <f t="array" aca="1" ref="L7" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Beef</v>
+        <v>Tuna</v>
       </c>
       <c r="M7" t="str" cm="1">
         <f t="array" aca="1" ref="M7" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Bread</v>
+        <v>Beef</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8">
+        <v>10</v>
+      </c>
+      <c r="E8">
+        <v>100</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9">
+        <v>10</v>
+      </c>
+      <c r="E9">
+        <v>100</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <v>10</v>
+      </c>
+      <c r="E10">
+        <v>100</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11">
+        <v>100</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>10</v>
+      </c>
+      <c r="E12">
+        <v>100</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13">
+        <v>10</v>
+      </c>
+      <c r="E13">
+        <v>100</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <v>10</v>
+      </c>
+      <c r="E14">
+        <v>100</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15">
+        <v>10</v>
+      </c>
+      <c r="E15">
+        <v>100</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C7" xr:uid="{22784EBF-D91C-4A9F-BBF6-DF997D832606}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C15" xr:uid="{22784EBF-D91C-4A9F-BBF6-DF997D832606}">
       <formula1>INDIRECT("ItemTypes[Type]")</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F7" xr:uid="{974DD810-82B8-4D7E-B93F-00E192FD871B}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F15" xr:uid="{974DD810-82B8-4D7E-B93F-00E192FD871B}">
       <formula1>1</formula1>
       <formula2>2</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4:E7" xr:uid="{F145B394-3EE5-45DA-BD07-F9070E8EDA1D}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4:E15" xr:uid="{F145B394-3EE5-45DA-BD07-F9070E8EDA1D}">
       <formula1>1</formula1>
       <formula2>100</formula2>
     </dataValidation>
@@ -720,23 +877,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="97dd5345-e793-494f-a61a-0ff5f2d8588d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EB9F34A24037AB4FA470085E68A4B53B" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1f05ce8c82e9282909648c3323760eae">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="97dd5345-e793-494f-a61a-0ff5f2d8588d" xmlns:ns4="72e2bb9d-dac6-4618-b85f-5ec835598a0c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c14bf05b446930f087596548c801372f" ns3:_="" ns4:_="">
     <xsd:import namespace="97dd5345-e793-494f-a61a-0ff5f2d8588d"/>
@@ -963,32 +1103,24 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="97dd5345-e793-494f-a61a-0ff5f2d8588d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA6B1F78-6D1D-4550-867C-D81A2584596E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="72e2bb9d-dac6-4618-b85f-5ec835598a0c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="97dd5345-e793-494f-a61a-0ff5f2d8588d"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB2BC082-80AE-42F8-9667-95CF6F1F5700}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{65537B17-CCB8-447E-A12B-556BEEDE4DB0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1005,4 +1137,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB2BC082-80AE-42F8-9667-95CF6F1F5700}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA6B1F78-6D1D-4550-867C-D81A2584596E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="72e2bb9d-dac6-4618-b85f-5ec835598a0c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="97dd5345-e793-494f-a61a-0ff5f2d8588d"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Modified spreadsheet with some changes
</commit_message>
<xml_diff>
--- a/UntitledKitchenGame/Game/UntitledKitchenGame/Assets/Editor/Items.xlsx
+++ b/UntitledKitchenGame/Game/UntitledKitchenGame/Assets/Editor/Items.xlsx
@@ -8,15 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\murra\OneDrive\Documents\GitHub\UntitledKitchenGame\UntitledKitchenGame\Game\UntitledKitchenGame\Assets\Editor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAAA3217-95A4-4E24-8D82-9D934CCF6513}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBB1CA2C-29E4-40FF-B4EE-1FD636C92ED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F8B15126-9F65-4AA0-BFBE-7FC0EBE8032D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F8B15126-9F65-4AA0-BFBE-7FC0EBE8032D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="ItemType">ItemTypes[[#Headers],[Type]]</definedName>
+    <definedName name="OrderIncludes">Sheet1!$U$2</definedName>
+    <definedName name="OrderIncludes2">Sheet1!$V$2</definedName>
+    <definedName name="OrderIncludes3">Sheet1!$W$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +42,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -61,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
   <si>
     <t>Points</t>
   </si>
@@ -136,6 +139,21 @@
   </si>
   <si>
     <t>Lettuce</t>
+  </si>
+  <si>
+    <t>Items</t>
+  </si>
+  <si>
+    <t>New Item</t>
+  </si>
+  <si>
+    <t>Final Slot</t>
+  </si>
+  <si>
+    <t>Experiements?</t>
+  </si>
+  <si>
+    <t>Order Includes…</t>
   </si>
 </sst>
 </file>
@@ -159,7 +177,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -167,15 +185,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -546,19 +580,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2334730F-D581-4249-91BD-F969B819BCBB}">
-  <dimension ref="B3:M15"/>
+  <dimension ref="B1:Z15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="U16" sqref="U16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" customWidth="1"/>
+    <col min="8" max="18" width="9.42578125" customWidth="1"/>
+    <col min="24" max="24" width="42.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J1" t="s">
+        <v>25</v>
+      </c>
+      <c r="U1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J2" t="s">
+        <v>27</v>
+      </c>
+      <c r="S2" t="s">
+        <v>26</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
@@ -577,20 +640,20 @@
       <c r="H3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="T3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="U3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="V3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="W3" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>9</v>
       </c>
@@ -609,20 +672,64 @@
       <c r="H4" t="s">
         <v>4</v>
       </c>
-      <c r="K4" t="str" cm="1">
-        <f t="array" aca="1" ref="K4" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Beef</v>
-      </c>
-      <c r="L4" t="str" cm="1">
-        <f t="array" aca="1" ref="L4" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
+      <c r="K4">
+        <f>L3</f>
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <f t="shared" ref="K4:N12" si="0">M3</f>
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <f t="shared" ref="O4:R12" si="1">P3</f>
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <f>S3</f>
+        <v>0</v>
+      </c>
+      <c r="S4" t="str" cm="1">
+        <f t="array" aca="1" ref="S4" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
+        <v>Tuna</v>
+      </c>
+      <c r="U4" t="str" cm="1">
+        <f t="array" aca="1" ref="U4" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
+        <v>Tuna</v>
+      </c>
+      <c r="V4" t="str" cm="1">
+        <f t="array" aca="1" ref="V4" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
+        <v>Rice</v>
+      </c>
+      <c r="W4" t="str" cm="1">
+        <f t="array" aca="1" ref="W4" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
         <v>Lobster</v>
       </c>
-      <c r="M4" t="str" cm="1">
-        <f t="array" aca="1" ref="M4" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Bread</v>
+      <c r="X4" t="str">
+        <f ca="1">_xlfn.CONCAT(J4:S4)</f>
+        <v>00000000Tuna</v>
+      </c>
+      <c r="Y4" t="e">
+        <f ca="1">IF((U4+V4+W4) = X4, TRUE,FALSE)</f>
+        <v>#VALUE!</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>19</v>
       </c>
@@ -641,20 +748,68 @@
       <c r="H5" t="s">
         <v>5</v>
       </c>
-      <c r="K5" t="str" cm="1">
-        <f t="array" aca="1" ref="K5" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
+      <c r="K5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <f>R4</f>
+        <v>0</v>
+      </c>
+      <c r="R5" t="str">
+        <f ca="1">S4</f>
+        <v>Tuna</v>
+      </c>
+      <c r="S5" t="str" cm="1">
+        <f t="array" aca="1" ref="S5" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
+        <v>Bread</v>
+      </c>
+      <c r="U5" t="str" cm="1">
+        <f t="array" aca="1" ref="U5" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
+        <v>Beef</v>
+      </c>
+      <c r="V5" t="str" cm="1">
+        <f t="array" aca="1" ref="V5" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
+        <v>Lettuce</v>
+      </c>
+      <c r="W5" t="str" cm="1">
+        <f t="array" aca="1" ref="W5" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
         <v>Rice</v>
       </c>
-      <c r="L5" t="str" cm="1">
-        <f t="array" aca="1" ref="L5" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Pork</v>
-      </c>
-      <c r="M5" t="str" cm="1">
-        <f t="array" aca="1" ref="M5" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Beef</v>
+      <c r="X5" t="str">
+        <f t="shared" ref="X5:X7" ca="1" si="2">_xlfn.CONCAT(J5:S5)</f>
+        <v>0000000TunaBread</v>
+      </c>
+      <c r="Y5">
+        <f ca="1">COUNTIF($J4:$S4, OR(U4,V4,W4))</f>
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <f ca="1">COUNTIF($J5:$S5, U5) +COUNTIF($J5:$S5, V5) + COUNTIF($J5:$S5,W5)</f>
+        <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>20</v>
       </c>
@@ -673,20 +828,64 @@
       <c r="H6" t="s">
         <v>6</v>
       </c>
-      <c r="K6" t="str" cm="1">
-        <f t="array" aca="1" ref="K6" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
+      <c r="K6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q6" t="str">
+        <f ca="1">R5</f>
         <v>Tuna</v>
       </c>
-      <c r="L6" t="str" cm="1">
-        <f t="array" aca="1" ref="L6" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Rice</v>
-      </c>
-      <c r="M6" t="str" cm="1">
-        <f t="array" aca="1" ref="M6" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Tuna</v>
+      <c r="R6" t="str">
+        <f ca="1">S5</f>
+        <v>Bread</v>
+      </c>
+      <c r="S6" t="str" cm="1">
+        <f t="array" aca="1" ref="S6" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
+        <v>Lettuce</v>
+      </c>
+      <c r="U6" t="str" cm="1">
+        <f t="array" aca="1" ref="U6" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
+        <v>Pork</v>
+      </c>
+      <c r="V6" t="str" cm="1">
+        <f t="array" aca="1" ref="V6" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
+        <v>Lobster</v>
+      </c>
+      <c r="W6" t="str" cm="1">
+        <f t="array" aca="1" ref="W6" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
+        <v>Lobster</v>
+      </c>
+      <c r="X6" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>000000TunaBreadLettuce</v>
+      </c>
+      <c r="Z6">
+        <f t="shared" ref="Z6:Z13" ca="1" si="3">COUNTIF($J6:$S6, U6) +COUNTIF($J6:$S6, V6) + COUNTIF($J6:$S6,W6)</f>
+        <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>11</v>
       </c>
@@ -705,20 +904,64 @@
       <c r="H7" t="s">
         <v>10</v>
       </c>
-      <c r="K7" t="str" cm="1">
-        <f t="array" aca="1" ref="K7" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Rice</v>
-      </c>
-      <c r="L7" t="str" cm="1">
-        <f t="array" aca="1" ref="L7" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
+      <c r="K7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P7" t="str">
+        <f t="shared" ca="1" si="1"/>
         <v>Tuna</v>
       </c>
-      <c r="M7" t="str" cm="1">
-        <f t="array" aca="1" ref="M7" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Beef</v>
+      <c r="Q7" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Bread</v>
+      </c>
+      <c r="R7" t="str">
+        <f ca="1">S6</f>
+        <v>Lettuce</v>
+      </c>
+      <c r="S7" t="str" cm="1">
+        <f t="array" aca="1" ref="S7" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
+        <v>Lettuce</v>
+      </c>
+      <c r="U7" t="str" cm="1">
+        <f t="array" aca="1" ref="U7" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
+        <v>Carrot</v>
+      </c>
+      <c r="V7" t="str" cm="1">
+        <f t="array" aca="1" ref="V7" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
+        <v>Chicken</v>
+      </c>
+      <c r="W7" t="str" cm="1">
+        <f t="array" aca="1" ref="W7" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
+        <v>Pasta</v>
+      </c>
+      <c r="X7" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>00000TunaBreadLettuceLettuce</v>
+      </c>
+      <c r="Z7">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>21</v>
       </c>
@@ -734,8 +977,60 @@
       <c r="F8">
         <v>1</v>
       </c>
+      <c r="K8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O8" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Tuna</v>
+      </c>
+      <c r="P8" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Bread</v>
+      </c>
+      <c r="Q8" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Lettuce</v>
+      </c>
+      <c r="R8" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Lettuce</v>
+      </c>
+      <c r="S8" t="str" cm="1">
+        <f t="array" aca="1" ref="S8" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
+        <v>Bread</v>
+      </c>
+      <c r="U8" t="str" cm="1">
+        <f t="array" aca="1" ref="U8" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
+        <v>Lobster</v>
+      </c>
+      <c r="V8" t="str" cm="1">
+        <f t="array" aca="1" ref="V8" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
+        <v>Lettuce</v>
+      </c>
+      <c r="W8" t="str" cm="1">
+        <f t="array" aca="1" ref="W8" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
+        <v>Salmon</v>
+      </c>
+      <c r="Z8">
+        <f ca="1">COUNTIF($J8:$S8, U8) +COUNTIF($J8:$S8, V8) + COUNTIF($J8:$S8,W8)</f>
+        <v>2</v>
+      </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>22</v>
       </c>
@@ -751,8 +1046,60 @@
       <c r="F9">
         <v>1</v>
       </c>
+      <c r="K9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N9" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Tuna</v>
+      </c>
+      <c r="O9" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Bread</v>
+      </c>
+      <c r="P9" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Lettuce</v>
+      </c>
+      <c r="Q9" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Lettuce</v>
+      </c>
+      <c r="R9" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Bread</v>
+      </c>
+      <c r="S9" t="str" cm="1">
+        <f t="array" aca="1" ref="S9" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
+        <v>Pasta</v>
+      </c>
+      <c r="U9" t="str" cm="1">
+        <f t="array" aca="1" ref="U9" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
+        <v>Pasta</v>
+      </c>
+      <c r="V9" t="str" cm="1">
+        <f t="array" aca="1" ref="V9" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
+        <v>Salmon</v>
+      </c>
+      <c r="W9" t="str" cm="1">
+        <f t="array" aca="1" ref="W9" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
+        <v>Salmon</v>
+      </c>
+      <c r="Z9">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>7</v>
       </c>
@@ -768,8 +1115,60 @@
       <c r="F10">
         <v>1</v>
       </c>
+      <c r="K10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M10" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Tuna</v>
+      </c>
+      <c r="N10" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Bread</v>
+      </c>
+      <c r="O10" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Lettuce</v>
+      </c>
+      <c r="P10" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Lettuce</v>
+      </c>
+      <c r="Q10" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Bread</v>
+      </c>
+      <c r="R10" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Pasta</v>
+      </c>
+      <c r="S10" t="str" cm="1">
+        <f t="array" aca="1" ref="S10" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
+        <v>Bread</v>
+      </c>
+      <c r="U10" t="str" cm="1">
+        <f t="array" aca="1" ref="U10" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
+        <v>Lettuce</v>
+      </c>
+      <c r="V10" t="str" cm="1">
+        <f t="array" aca="1" ref="V10" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
+        <v>Bread</v>
+      </c>
+      <c r="W10" t="str" cm="1">
+        <f t="array" aca="1" ref="W10" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
+        <v>Carrot</v>
+      </c>
+      <c r="Z10">
+        <f t="shared" ca="1" si="3"/>
+        <v>5</v>
+      </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>17</v>
       </c>
@@ -785,8 +1184,60 @@
       <c r="F11">
         <v>1</v>
       </c>
+      <c r="K11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L11" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Tuna</v>
+      </c>
+      <c r="M11" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Bread</v>
+      </c>
+      <c r="N11" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Lettuce</v>
+      </c>
+      <c r="O11" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Lettuce</v>
+      </c>
+      <c r="P11" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Bread</v>
+      </c>
+      <c r="Q11" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Pasta</v>
+      </c>
+      <c r="R11" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Bread</v>
+      </c>
+      <c r="S11" t="str" cm="1">
+        <f t="array" aca="1" ref="S11" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
+        <v>Pork</v>
+      </c>
+      <c r="U11" t="str" cm="1">
+        <f t="array" aca="1" ref="U11" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
+        <v>Onion</v>
+      </c>
+      <c r="V11" t="str" cm="1">
+        <f t="array" aca="1" ref="V11" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
+        <v>Carrot</v>
+      </c>
+      <c r="W11" t="str" cm="1">
+        <f t="array" aca="1" ref="W11" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
+        <v>Chicken</v>
+      </c>
+      <c r="Z11">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>18</v>
       </c>
@@ -802,8 +1253,60 @@
       <c r="F12">
         <v>1</v>
       </c>
+      <c r="K12" t="str">
+        <f ca="1">L11</f>
+        <v>Tuna</v>
+      </c>
+      <c r="L12" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Bread</v>
+      </c>
+      <c r="M12" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Lettuce</v>
+      </c>
+      <c r="N12" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Lettuce</v>
+      </c>
+      <c r="O12" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Bread</v>
+      </c>
+      <c r="P12" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Pasta</v>
+      </c>
+      <c r="Q12" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Bread</v>
+      </c>
+      <c r="R12" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Pork</v>
+      </c>
+      <c r="S12" t="str" cm="1">
+        <f t="array" aca="1" ref="S12" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
+        <v>Bread</v>
+      </c>
+      <c r="U12" t="str" cm="1">
+        <f t="array" aca="1" ref="U12" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
+        <v>Carrot</v>
+      </c>
+      <c r="V12" t="str" cm="1">
+        <f t="array" aca="1" ref="V12" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
+        <v>Chicken</v>
+      </c>
+      <c r="W12" t="str" cm="1">
+        <f t="array" aca="1" ref="W12" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
+        <v>Beef</v>
+      </c>
+      <c r="Z12">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>8</v>
       </c>
@@ -820,7 +1323,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>23</v>
       </c>
@@ -837,7 +1340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>24</v>
       </c>
@@ -852,11 +1355,23 @@
       </c>
       <c r="F15">
         <v>1</v>
+      </c>
+      <c r="U15" t="str" cm="1">
+        <f t="array" aca="1" ref="U15" ca="1">_xlfn.SINGLE(INDEX(_xlfn._xlws.FILTER(Food[],Food[Type] =OrderIncludes, "ERR"),RANDBETWEEN(0,3)))</f>
+        <v>Pasta</v>
+      </c>
+      <c r="V15" t="e" cm="1">
+        <f t="array" aca="1" ref="V15" ca="1">_xlfn.SINGLE(INDEX(_xlfn._xlws.FILTER(Food[],Food[Points] = OR(OrderIncludes,OrderIncludes2,OrderIncludes3), "ERR"),RANDBETWEEN(0,3)))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="W15" t="e" cm="1">
+        <f t="array" aca="1" ref="W15" ca="1">_xlfn.SINGLE(INDEX(_xlfn._xlws.FILTER(Food[],Food[Type] =NOT(OrderIncludes), "ERR"),RANDBETWEEN(0,3)))</f>
+        <v>#VALUE!</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C15" xr:uid="{22784EBF-D91C-4A9F-BBF6-DF997D832606}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C15 U2:W2" xr:uid="{22784EBF-D91C-4A9F-BBF6-DF997D832606}">
       <formula1>INDIRECT("ItemTypes[Type]")</formula1>
     </dataValidation>
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F15" xr:uid="{974DD810-82B8-4D7E-B93F-00E192FD871B}">
@@ -877,6 +1392,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="97dd5345-e793-494f-a61a-0ff5f2d8588d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EB9F34A24037AB4FA470085E68A4B53B" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1f05ce8c82e9282909648c3323760eae">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="97dd5345-e793-494f-a61a-0ff5f2d8588d" xmlns:ns4="72e2bb9d-dac6-4618-b85f-5ec835598a0c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c14bf05b446930f087596548c801372f" ns3:_="" ns4:_="">
     <xsd:import namespace="97dd5345-e793-494f-a61a-0ff5f2d8588d"/>
@@ -1103,24 +1635,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA6B1F78-6D1D-4550-867C-D81A2584596E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="72e2bb9d-dac6-4618-b85f-5ec835598a0c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="97dd5345-e793-494f-a61a-0ff5f2d8588d"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="97dd5345-e793-494f-a61a-0ff5f2d8588d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB2BC082-80AE-42F8-9667-95CF6F1F5700}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{65537B17-CCB8-447E-A12B-556BEEDE4DB0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1137,29 +1677,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB2BC082-80AE-42F8-9667-95CF6F1F5700}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA6B1F78-6D1D-4550-867C-D81A2584596E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="72e2bb9d-dac6-4618-b85f-5ec835598a0c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="97dd5345-e793-494f-a61a-0ff5f2d8588d"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Submitted my design jounral
Would lie to keep experimenting but am tired and need more questions
</commit_message>
<xml_diff>
--- a/UntitledKitchenGame/Game/UntitledKitchenGame/Assets/Editor/Items.xlsx
+++ b/UntitledKitchenGame/Game/UntitledKitchenGame/Assets/Editor/Items.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\murra\OneDrive\Documents\GitHub\UntitledKitchenGame\UntitledKitchenGame\Game\UntitledKitchenGame\Assets\Editor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBB1CA2C-29E4-40FF-B4EE-1FD636C92ED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7D7A5D6-AC63-48F5-904F-521BC09F2F63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F8B15126-9F65-4AA0-BFBE-7FC0EBE8032D}"/>
   </bookViews>
@@ -580,10 +580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2334730F-D581-4249-91BD-F969B819BCBB}">
-  <dimension ref="B1:Z15"/>
+  <dimension ref="B1:Z19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U16" sqref="U16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="X7" sqref="X7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -706,23 +706,23 @@
       </c>
       <c r="S4" t="str" cm="1">
         <f t="array" aca="1" ref="S4" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Tuna</v>
+        <v>Carrot</v>
       </c>
       <c r="U4" t="str" cm="1">
         <f t="array" aca="1" ref="U4" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Tuna</v>
-      </c>
-      <c r="V4" t="str" cm="1">
-        <f t="array" aca="1" ref="V4" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Rice</v>
+        <v>Bread</v>
+      </c>
+      <c r="V4" cm="1">
+        <f t="array" aca="1" ref="V4" ca="1">IF(INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))=U4,"-",RANDBETWEEN(1,COUNTA(Food[Name])))</f>
+        <v>6</v>
       </c>
       <c r="W4" t="str" cm="1">
         <f t="array" aca="1" ref="W4" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Lobster</v>
+        <v>Chicken</v>
       </c>
       <c r="X4" t="str">
         <f ca="1">_xlfn.CONCAT(J4:S4)</f>
-        <v>00000000Tuna</v>
+        <v>00000000Carrot</v>
       </c>
       <c r="Y4" t="e">
         <f ca="1">IF((U4+V4+W4) = X4, TRUE,FALSE)</f>
@@ -778,27 +778,27 @@
       </c>
       <c r="R5" t="str">
         <f ca="1">S4</f>
-        <v>Tuna</v>
+        <v>Carrot</v>
       </c>
       <c r="S5" t="str" cm="1">
         <f t="array" aca="1" ref="S5" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Bread</v>
+        <v>Pasta</v>
       </c>
       <c r="U5" t="str" cm="1">
         <f t="array" aca="1" ref="U5" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Beef</v>
+        <v>Pasta</v>
       </c>
       <c r="V5" t="str" cm="1">
         <f t="array" aca="1" ref="V5" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Lettuce</v>
+        <v>Rice</v>
       </c>
       <c r="W5" t="str" cm="1">
         <f t="array" aca="1" ref="W5" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Rice</v>
+        <v>Bread</v>
       </c>
       <c r="X5" t="str">
         <f t="shared" ref="X5:X7" ca="1" si="2">_xlfn.CONCAT(J5:S5)</f>
-        <v>0000000TunaBread</v>
+        <v>0000000CarrotPasta</v>
       </c>
       <c r="Y5">
         <f ca="1">COUNTIF($J4:$S4, OR(U4,V4,W4))</f>
@@ -806,7 +806,7 @@
       </c>
       <c r="Z5">
         <f ca="1">COUNTIF($J5:$S5, U5) +COUNTIF($J5:$S5, V5) + COUNTIF($J5:$S5,W5)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:26" x14ac:dyDescent="0.25">
@@ -854,11 +854,11 @@
       </c>
       <c r="Q6" t="str">
         <f ca="1">R5</f>
-        <v>Tuna</v>
+        <v>Carrot</v>
       </c>
       <c r="R6" t="str">
         <f ca="1">S5</f>
-        <v>Bread</v>
+        <v>Pasta</v>
       </c>
       <c r="S6" t="str" cm="1">
         <f t="array" aca="1" ref="S6" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
@@ -866,19 +866,19 @@
       </c>
       <c r="U6" t="str" cm="1">
         <f t="array" aca="1" ref="U6" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Pork</v>
+        <v>Salmon</v>
       </c>
       <c r="V6" t="str" cm="1">
         <f t="array" aca="1" ref="V6" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Lobster</v>
+        <v>Rice</v>
       </c>
       <c r="W6" t="str" cm="1">
         <f t="array" aca="1" ref="W6" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Lobster</v>
+        <v>Beef</v>
       </c>
       <c r="X6" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>000000TunaBreadLettuce</v>
+        <v>000000CarrotPastaLettuce</v>
       </c>
       <c r="Z6">
         <f t="shared" ref="Z6:Z13" ca="1" si="3">COUNTIF($J6:$S6, U6) +COUNTIF($J6:$S6, V6) + COUNTIF($J6:$S6,W6)</f>
@@ -926,11 +926,11 @@
       </c>
       <c r="P7" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Tuna</v>
+        <v>Carrot</v>
       </c>
       <c r="Q7" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Bread</v>
+        <v>Pasta</v>
       </c>
       <c r="R7" t="str">
         <f ca="1">S6</f>
@@ -938,27 +938,15 @@
       </c>
       <c r="S7" t="str" cm="1">
         <f t="array" aca="1" ref="S7" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Lettuce</v>
-      </c>
-      <c r="U7" t="str" cm="1">
-        <f t="array" aca="1" ref="U7" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Carrot</v>
-      </c>
-      <c r="V7" t="str" cm="1">
-        <f t="array" aca="1" ref="V7" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
         <v>Chicken</v>
       </c>
-      <c r="W7" t="str" cm="1">
-        <f t="array" aca="1" ref="W7" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Pasta</v>
-      </c>
       <c r="X7" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>00000TunaBreadLettuceLettuce</v>
+        <f ca="1">_xlfn.CONCAT(J7:S7)</f>
+        <v>00000CarrotPastaLettuceChicken</v>
       </c>
       <c r="Z7">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="2:26" x14ac:dyDescent="0.25">
@@ -995,11 +983,11 @@
       </c>
       <c r="O8" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Tuna</v>
+        <v>Carrot</v>
       </c>
       <c r="P8" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Bread</v>
+        <v>Pasta</v>
       </c>
       <c r="Q8" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -1007,27 +995,11 @@
       </c>
       <c r="R8" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Lettuce</v>
+        <v>Chicken</v>
       </c>
       <c r="S8" t="str" cm="1">
         <f t="array" aca="1" ref="S8" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Bread</v>
-      </c>
-      <c r="U8" t="str" cm="1">
-        <f t="array" aca="1" ref="U8" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Lobster</v>
-      </c>
-      <c r="V8" t="str" cm="1">
-        <f t="array" aca="1" ref="V8" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Lettuce</v>
-      </c>
-      <c r="W8" t="str" cm="1">
-        <f t="array" aca="1" ref="W8" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Salmon</v>
-      </c>
-      <c r="Z8">
-        <f ca="1">COUNTIF($J8:$S8, U8) +COUNTIF($J8:$S8, V8) + COUNTIF($J8:$S8,W8)</f>
-        <v>2</v>
+        <v>Beef</v>
       </c>
     </row>
     <row r="9" spans="2:26" x14ac:dyDescent="0.25">
@@ -1060,11 +1032,11 @@
       </c>
       <c r="N9" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Tuna</v>
+        <v>Carrot</v>
       </c>
       <c r="O9" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Bread</v>
+        <v>Pasta</v>
       </c>
       <c r="P9" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -1072,31 +1044,15 @@
       </c>
       <c r="Q9" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Lettuce</v>
+        <v>Chicken</v>
       </c>
       <c r="R9" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Bread</v>
+        <v>Beef</v>
       </c>
       <c r="S9" t="str" cm="1">
         <f t="array" aca="1" ref="S9" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Pasta</v>
-      </c>
-      <c r="U9" t="str" cm="1">
-        <f t="array" aca="1" ref="U9" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Pasta</v>
-      </c>
-      <c r="V9" t="str" cm="1">
-        <f t="array" aca="1" ref="V9" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Salmon</v>
-      </c>
-      <c r="W9" t="str" cm="1">
-        <f t="array" aca="1" ref="W9" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Salmon</v>
-      </c>
-      <c r="Z9">
-        <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>Onion</v>
       </c>
     </row>
     <row r="10" spans="2:26" x14ac:dyDescent="0.25">
@@ -1125,11 +1081,11 @@
       </c>
       <c r="M10" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Tuna</v>
+        <v>Carrot</v>
       </c>
       <c r="N10" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Bread</v>
+        <v>Pasta</v>
       </c>
       <c r="O10" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -1137,35 +1093,19 @@
       </c>
       <c r="P10" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Lettuce</v>
+        <v>Chicken</v>
       </c>
       <c r="Q10" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Bread</v>
+        <v>Beef</v>
       </c>
       <c r="R10" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Pasta</v>
+        <v>Onion</v>
       </c>
       <c r="S10" t="str" cm="1">
         <f t="array" aca="1" ref="S10" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Bread</v>
-      </c>
-      <c r="U10" t="str" cm="1">
-        <f t="array" aca="1" ref="U10" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Lettuce</v>
-      </c>
-      <c r="V10" t="str" cm="1">
-        <f t="array" aca="1" ref="V10" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Bread</v>
-      </c>
-      <c r="W10" t="str" cm="1">
-        <f t="array" aca="1" ref="W10" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Carrot</v>
-      </c>
-      <c r="Z10">
-        <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>Pasta</v>
       </c>
     </row>
     <row r="11" spans="2:26" x14ac:dyDescent="0.25">
@@ -1190,11 +1130,11 @@
       </c>
       <c r="L11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Tuna</v>
+        <v>Carrot</v>
       </c>
       <c r="M11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Bread</v>
+        <v>Pasta</v>
       </c>
       <c r="N11" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -1202,39 +1142,23 @@
       </c>
       <c r="O11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Lettuce</v>
+        <v>Chicken</v>
       </c>
       <c r="P11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Bread</v>
+        <v>Beef</v>
       </c>
       <c r="Q11" t="str">
         <f t="shared" ca="1" si="1"/>
+        <v>Onion</v>
+      </c>
+      <c r="R11" t="str">
+        <f t="shared" ca="1" si="1"/>
         <v>Pasta</v>
-      </c>
-      <c r="R11" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Bread</v>
       </c>
       <c r="S11" t="str" cm="1">
         <f t="array" aca="1" ref="S11" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Pork</v>
-      </c>
-      <c r="U11" t="str" cm="1">
-        <f t="array" aca="1" ref="U11" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Onion</v>
-      </c>
-      <c r="V11" t="str" cm="1">
-        <f t="array" aca="1" ref="V11" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
         <v>Carrot</v>
-      </c>
-      <c r="W11" t="str" cm="1">
-        <f t="array" aca="1" ref="W11" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Chicken</v>
-      </c>
-      <c r="Z11">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:26" x14ac:dyDescent="0.25">
@@ -1255,11 +1179,11 @@
       </c>
       <c r="K12" t="str">
         <f ca="1">L11</f>
-        <v>Tuna</v>
+        <v>Carrot</v>
       </c>
       <c r="L12" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Bread</v>
+        <v>Pasta</v>
       </c>
       <c r="M12" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -1267,44 +1191,28 @@
       </c>
       <c r="N12" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Lettuce</v>
+        <v>Chicken</v>
       </c>
       <c r="O12" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Bread</v>
+        <v>Beef</v>
       </c>
       <c r="P12" t="str">
         <f t="shared" ca="1" si="1"/>
+        <v>Onion</v>
+      </c>
+      <c r="Q12" t="str">
+        <f t="shared" ca="1" si="1"/>
         <v>Pasta</v>
       </c>
-      <c r="Q12" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Bread</v>
-      </c>
       <c r="R12" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Pork</v>
+        <v>Carrot</v>
       </c>
       <c r="S12" t="str" cm="1">
         <f t="array" aca="1" ref="S12" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
         <v>Bread</v>
       </c>
-      <c r="U12" t="str" cm="1">
-        <f t="array" aca="1" ref="U12" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Carrot</v>
-      </c>
-      <c r="V12" t="str" cm="1">
-        <f t="array" aca="1" ref="V12" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Chicken</v>
-      </c>
-      <c r="W12" t="str" cm="1">
-        <f t="array" aca="1" ref="W12" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Beef</v>
-      </c>
-      <c r="Z12">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="13" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
@@ -1356,9 +1264,9 @@
       <c r="F15">
         <v>1</v>
       </c>
-      <c r="U15" t="str" cm="1">
-        <f t="array" aca="1" ref="U15" ca="1">_xlfn.SINGLE(INDEX(_xlfn._xlws.FILTER(Food[],Food[Type] =OrderIncludes, "ERR"),RANDBETWEEN(0,3)))</f>
-        <v>Pasta</v>
+      <c r="U15" t="e" cm="1">
+        <f t="array" aca="1" ref="U15" ca="1">_xlfn.SINGLE(INDEX(_xlfn._xlws.FILTER(Food[],Food[Type]=OrderIncludes,"ERR"),RANDBETWEEN(0,COUNTA(Food[Type]))))</f>
+        <v>#REF!</v>
       </c>
       <c r="V15" t="e" cm="1">
         <f t="array" aca="1" ref="V15" ca="1">_xlfn.SINGLE(INDEX(_xlfn._xlws.FILTER(Food[],Food[Points] = OR(OrderIncludes,OrderIncludes2,OrderIncludes3), "ERR"),RANDBETWEEN(0,3)))</f>
@@ -1367,6 +1275,58 @@
       <c r="W15" t="e" cm="1">
         <f t="array" aca="1" ref="W15" ca="1">_xlfn.SINGLE(INDEX(_xlfn._xlws.FILTER(Food[],Food[Type] =NOT(OrderIncludes), "ERR"),RANDBETWEEN(0,3)))</f>
         <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="17" spans="21:25" x14ac:dyDescent="0.25">
+      <c r="U17" t="str" cm="1">
+        <f t="array" ref="U17:Y19">_xlfn._xlws.FILTER(Food[],Food[Type]=OrderIncludes,"ERR")</f>
+        <v>Bread</v>
+      </c>
+      <c r="V17" t="str">
+        <v>Grain</v>
+      </c>
+      <c r="W17">
+        <v>10</v>
+      </c>
+      <c r="X17">
+        <v>100</v>
+      </c>
+      <c r="Y17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="21:25" x14ac:dyDescent="0.25">
+      <c r="U18" t="str">
+        <v>Pasta</v>
+      </c>
+      <c r="V18" t="str">
+        <v>Grain</v>
+      </c>
+      <c r="W18">
+        <v>10</v>
+      </c>
+      <c r="X18">
+        <v>100</v>
+      </c>
+      <c r="Y18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="21:25" x14ac:dyDescent="0.25">
+      <c r="U19" t="str">
+        <v>Rice</v>
+      </c>
+      <c r="V19" t="str">
+        <v>Grain</v>
+      </c>
+      <c r="W19">
+        <v>10</v>
+      </c>
+      <c r="X19">
+        <v>100</v>
+      </c>
+      <c r="Y19">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modifications after the checkin with teach
</commit_message>
<xml_diff>
--- a/UntitledKitchenGame/Game/UntitledKitchenGame/Assets/Editor/Items.xlsx
+++ b/UntitledKitchenGame/Game/UntitledKitchenGame/Assets/Editor/Items.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\murra\OneDrive\Documents\GitHub\UntitledKitchenGame\UntitledKitchenGame\Game\UntitledKitchenGame\Assets\Editor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\placej\source\repos\UntitledKitchenGame\UntitledKitchenGame\Game\UntitledKitchenGame\Assets\Editor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{788A8F60-8854-46FB-8385-C1583308EFE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D015D257-0390-4DDD-BBA0-2B2FB9878E41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F8B15126-9F65-4AA0-BFBE-7FC0EBE8032D}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{F8B15126-9F65-4AA0-BFBE-7FC0EBE8032D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -166,7 +166,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -589,17 +589,17 @@
   <dimension ref="B1:Z22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="R23" sqref="R23"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="18" width="9.42578125" customWidth="1"/>
-    <col min="24" max="24" width="42.140625" customWidth="1"/>
+    <col min="5" max="5" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="18" width="9.375" customWidth="1"/>
+    <col min="24" max="24" width="42.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:26" ht="15" thickBot="1">
       <c r="J1" t="s">
         <v>25</v>
       </c>
@@ -607,7 +607,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:26" ht="15" thickBot="1">
       <c r="J2" t="s">
         <v>27</v>
       </c>
@@ -627,7 +627,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:26" s="1" customFormat="1">
       <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
@@ -659,7 +659,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:26">
       <c r="B4" t="s">
         <v>9</v>
       </c>
@@ -712,30 +712,30 @@
       </c>
       <c r="S4" t="str" cm="1">
         <f t="array" aca="1" ref="S4" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Chicken</v>
+        <v>Beef</v>
       </c>
       <c r="U4" t="str" cm="1">
         <f t="array" aca="1" ref="U4" ca="1">IF(INDEX(Food[Name],OrderIndex)= OR(OrderIndex2,OrderIndex3),"FirstConTrue", INDEX(Food[Name],OrderIndex))</f>
-        <v>Beef</v>
+        <v>Chicken</v>
       </c>
       <c r="V4" t="str" cm="1">
         <f t="array" aca="1" ref="V4" ca="1">IF(INDEX(Food[Name],OrderIndex2)= OR(OrderIndex,OrderIndex3),"FirstConTrue", INDEX(Food[Name],OrderIndex2))</f>
-        <v>Carrot</v>
+        <v>Tuna</v>
       </c>
       <c r="W4" t="str" cm="1">
         <f t="array" aca="1" ref="W4" ca="1">IF(INDEX(Food[Name],OrderIndex3)= OR(OrderIndex2,OrderIndex),"FirstConTrue", INDEX(Food[Name],OrderIndex3))</f>
-        <v>Beef</v>
+        <v>Tuna</v>
       </c>
       <c r="X4" t="str">
         <f ca="1">_xlfn.CONCAT(J4:S4)</f>
-        <v>00000000Chicken</v>
+        <v>00000000Beef</v>
       </c>
       <c r="Y4" t="e">
         <f ca="1">IF((U4+V4+W4) = X4, TRUE,FALSE)</f>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="5" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:26">
       <c r="B5" t="s">
         <v>19</v>
       </c>
@@ -784,27 +784,27 @@
       </c>
       <c r="R5" t="str">
         <f ca="1">S4</f>
-        <v>Chicken</v>
+        <v>Beef</v>
       </c>
       <c r="S5" t="str" cm="1">
         <f t="array" aca="1" ref="S5" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Salmon</v>
+        <v>Beef</v>
       </c>
       <c r="U5" t="str" cm="1">
         <f t="array" aca="1" ref="U5" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Lobster</v>
+        <v>Tuna</v>
       </c>
       <c r="V5" t="str" cm="1">
         <f t="array" aca="1" ref="V5" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Bread</v>
+        <v>Lettuce</v>
       </c>
       <c r="W5" t="str" cm="1">
         <f t="array" aca="1" ref="W5" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Tuna</v>
+        <v>Chicken</v>
       </c>
       <c r="X5" t="str">
-        <f t="shared" ref="X5:X7" ca="1" si="2">_xlfn.CONCAT(J5:S5)</f>
-        <v>0000000ChickenSalmon</v>
+        <f t="shared" ref="X5:X6" ca="1" si="2">_xlfn.CONCAT(J5:S5)</f>
+        <v>0000000BeefBeef</v>
       </c>
       <c r="Y5">
         <f ca="1">COUNTIF($J4:$S4, OR(U4,V4,W4))</f>
@@ -815,7 +815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:26">
       <c r="B6" t="s">
         <v>20</v>
       </c>
@@ -860,38 +860,38 @@
       </c>
       <c r="Q6" t="str">
         <f ca="1">R5</f>
-        <v>Chicken</v>
+        <v>Beef</v>
       </c>
       <c r="R6" t="str">
         <f ca="1">S5</f>
-        <v>Salmon</v>
+        <v>Beef</v>
       </c>
       <c r="S6" t="str" cm="1">
         <f t="array" aca="1" ref="S6" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Pasta</v>
+        <v>Salmon</v>
       </c>
       <c r="U6" t="str" cm="1">
         <f t="array" aca="1" ref="U6" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Pasta</v>
+        <v>Onion</v>
       </c>
       <c r="V6" t="str" cm="1">
         <f t="array" aca="1" ref="V6" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Lobster</v>
+        <v>Onion</v>
       </c>
       <c r="W6" t="str" cm="1">
         <f t="array" aca="1" ref="W6" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Pasta</v>
+        <v>Bread</v>
       </c>
       <c r="X6" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>000000ChickenSalmonPasta</v>
+        <v>000000BeefBeefSalmon</v>
       </c>
       <c r="Z6">
-        <f t="shared" ref="Z6:Z13" ca="1" si="3">COUNTIF($J6:$S6, U6) +COUNTIF($J6:$S6, V6) + COUNTIF($J6:$S6,W6)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="2:26" x14ac:dyDescent="0.25">
+        <f t="shared" ref="Z6:Z7" ca="1" si="3">COUNTIF($J6:$S6, U6) +COUNTIF($J6:$S6, V6) + COUNTIF($J6:$S6,W6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:26">
       <c r="B7" t="s">
         <v>11</v>
       </c>
@@ -932,30 +932,30 @@
       </c>
       <c r="P7" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Chicken</v>
+        <v>Beef</v>
       </c>
       <c r="Q7" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Salmon</v>
+        <v>Beef</v>
       </c>
       <c r="R7" t="str">
         <f ca="1">S6</f>
-        <v>Pasta</v>
+        <v>Salmon</v>
       </c>
       <c r="S7" t="str" cm="1">
         <f t="array" aca="1" ref="S7" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Pork</v>
+        <v>Beef</v>
       </c>
       <c r="X7" t="str">
         <f ca="1">_xlfn.CONCAT(J7:S7)</f>
-        <v>00000ChickenSalmonPastaPork</v>
+        <v>00000BeefBeefSalmonBeef</v>
       </c>
       <c r="Z7">
         <f t="shared" ca="1" si="3"/>
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:26">
       <c r="B8" t="s">
         <v>21</v>
       </c>
@@ -989,26 +989,26 @@
       </c>
       <c r="O8" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Chicken</v>
+        <v>Beef</v>
       </c>
       <c r="P8" t="str">
         <f t="shared" ca="1" si="1"/>
+        <v>Beef</v>
+      </c>
+      <c r="Q8" t="str">
+        <f t="shared" ca="1" si="1"/>
         <v>Salmon</v>
       </c>
-      <c r="Q8" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Pasta</v>
-      </c>
       <c r="R8" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Pork</v>
+        <v>Beef</v>
       </c>
       <c r="S8" t="str" cm="1">
         <f t="array" aca="1" ref="S8" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Pasta</v>
-      </c>
-    </row>
-    <row r="9" spans="2:26" x14ac:dyDescent="0.25">
+        <v>Beef</v>
+      </c>
+    </row>
+    <row r="9" spans="2:26">
       <c r="B9" t="s">
         <v>22</v>
       </c>
@@ -1038,30 +1038,30 @@
       </c>
       <c r="N9" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Chicken</v>
+        <v>Beef</v>
       </c>
       <c r="O9" t="str">
         <f t="shared" ca="1" si="1"/>
+        <v>Beef</v>
+      </c>
+      <c r="P9" t="str">
+        <f t="shared" ca="1" si="1"/>
         <v>Salmon</v>
       </c>
-      <c r="P9" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Pasta</v>
-      </c>
       <c r="Q9" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Pork</v>
+        <v>Beef</v>
       </c>
       <c r="R9" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Pasta</v>
+        <v>Beef</v>
       </c>
       <c r="S9" t="str" cm="1">
         <f t="array" aca="1" ref="S9" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Onion</v>
-      </c>
-    </row>
-    <row r="10" spans="2:26" x14ac:dyDescent="0.25">
+        <v>Pasta</v>
+      </c>
+    </row>
+    <row r="10" spans="2:26">
       <c r="B10" t="s">
         <v>7</v>
       </c>
@@ -1087,34 +1087,34 @@
       </c>
       <c r="M10" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Chicken</v>
+        <v>Beef</v>
       </c>
       <c r="N10" t="str">
         <f t="shared" ca="1" si="0"/>
+        <v>Beef</v>
+      </c>
+      <c r="O10" t="str">
+        <f t="shared" ca="1" si="1"/>
         <v>Salmon</v>
       </c>
-      <c r="O10" t="str">
+      <c r="P10" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Beef</v>
+      </c>
+      <c r="Q10" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Beef</v>
+      </c>
+      <c r="R10" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>Pasta</v>
-      </c>
-      <c r="P10" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Pork</v>
-      </c>
-      <c r="Q10" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Pasta</v>
-      </c>
-      <c r="R10" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Onion</v>
       </c>
       <c r="S10" t="str" cm="1">
         <f t="array" aca="1" ref="S10" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Lobster</v>
-      </c>
-    </row>
-    <row r="11" spans="2:26" x14ac:dyDescent="0.25">
+        <v>Onion</v>
+      </c>
+    </row>
+    <row r="11" spans="2:26">
       <c r="B11" t="s">
         <v>17</v>
       </c>
@@ -1136,38 +1136,38 @@
       </c>
       <c r="L11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Chicken</v>
+        <v>Beef</v>
       </c>
       <c r="M11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Salmon</v>
+        <v>Beef</v>
       </c>
       <c r="N11" t="str">
         <f t="shared" ca="1" si="0"/>
+        <v>Salmon</v>
+      </c>
+      <c r="O11" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Beef</v>
+      </c>
+      <c r="P11" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Beef</v>
+      </c>
+      <c r="Q11" t="str">
+        <f t="shared" ca="1" si="1"/>
         <v>Pasta</v>
       </c>
-      <c r="O11" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Pork</v>
-      </c>
-      <c r="P11" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Pasta</v>
-      </c>
-      <c r="Q11" t="str">
+      <c r="R11" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>Onion</v>
-      </c>
-      <c r="R11" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Lobster</v>
       </c>
       <c r="S11" t="str" cm="1">
         <f t="array" aca="1" ref="S11" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Rice</v>
-      </c>
-    </row>
-    <row r="12" spans="2:26" x14ac:dyDescent="0.25">
+        <v>Pasta</v>
+      </c>
+    </row>
+    <row r="12" spans="2:26">
       <c r="B12" t="s">
         <v>18</v>
       </c>
@@ -1185,42 +1185,42 @@
       </c>
       <c r="K12" t="str">
         <f ca="1">L11</f>
-        <v>Chicken</v>
+        <v>Beef</v>
       </c>
       <c r="L12" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Salmon</v>
+        <v>Beef</v>
       </c>
       <c r="M12" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Pasta</v>
+        <v>Salmon</v>
       </c>
       <c r="N12" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Pork</v>
+        <v>Beef</v>
       </c>
       <c r="O12" t="str">
         <f t="shared" ca="1" si="1"/>
+        <v>Beef</v>
+      </c>
+      <c r="P12" t="str">
+        <f t="shared" ca="1" si="1"/>
         <v>Pasta</v>
       </c>
-      <c r="P12" t="str">
+      <c r="Q12" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>Onion</v>
       </c>
-      <c r="Q12" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Lobster</v>
-      </c>
       <c r="R12" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Rice</v>
+        <v>Pasta</v>
       </c>
       <c r="S12" t="str" cm="1">
         <f t="array" aca="1" ref="S12" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Rice</v>
-      </c>
-    </row>
-    <row r="13" spans="2:26" x14ac:dyDescent="0.25">
+        <v>Lobster</v>
+      </c>
+    </row>
+    <row r="13" spans="2:26">
       <c r="B13" t="s">
         <v>8</v>
       </c>
@@ -1237,7 +1237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:26">
       <c r="B14" t="s">
         <v>23</v>
       </c>
@@ -1254,7 +1254,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:26">
       <c r="B15" t="s">
         <v>24</v>
       </c>
@@ -1283,7 +1283,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="17" spans="14:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="14:25">
       <c r="U17" t="str" cm="1">
         <f t="array" ref="U17:Y19">_xlfn._xlws.FILTER(Food[],Food[Type]=OrderIncludes,"ERR")</f>
         <v>Bread</v>
@@ -1301,7 +1301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="14:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="14:25">
       <c r="U18" t="str">
         <v>Pasta</v>
       </c>
@@ -1318,7 +1318,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="14:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="14:25">
       <c r="U19" t="str">
         <v>Rice</v>
       </c>
@@ -1335,27 +1335,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="14:25" x14ac:dyDescent="0.25">
+    <row r="21" spans="14:25">
       <c r="N21" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="14:25" x14ac:dyDescent="0.25">
+    <row r="22" spans="14:25">
       <c r="N22">
         <f ca="1">RANDBETWEEN(1,COUNTA(Food[Name]))</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="O22">
         <f ca="1">RANDBETWEEN(1,COUNTA(Food[Type]))</f>
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="P22">
         <f ca="1">RANDBETWEEN(1,COUNTA(Food[Points]))</f>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="R22" t="str" cm="1">
         <f t="array" aca="1" ref="R22" ca="1">IF(INDEX(Food[Name],OrderIndex2)= OR(OrderIndex,OrderIndex3), "-",INDEX(Food[Name],OrderIndex2))</f>
-        <v>Carrot</v>
+        <v>Tuna</v>
       </c>
     </row>
   </sheetData>
@@ -1381,23 +1381,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="97dd5345-e793-494f-a61a-0ff5f2d8588d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EB9F34A24037AB4FA470085E68A4B53B" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1f05ce8c82e9282909648c3323760eae">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="97dd5345-e793-494f-a61a-0ff5f2d8588d" xmlns:ns4="72e2bb9d-dac6-4618-b85f-5ec835598a0c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c14bf05b446930f087596548c801372f" ns3:_="" ns4:_="">
     <xsd:import namespace="97dd5345-e793-494f-a61a-0ff5f2d8588d"/>
@@ -1624,32 +1607,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA6B1F78-6D1D-4550-867C-D81A2584596E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="72e2bb9d-dac6-4618-b85f-5ec835598a0c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="97dd5345-e793-494f-a61a-0ff5f2d8588d"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB2BC082-80AE-42F8-9667-95CF6F1F5700}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="97dd5345-e793-494f-a61a-0ff5f2d8588d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{65537B17-CCB8-447E-A12B-556BEEDE4DB0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1666,4 +1641,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB2BC082-80AE-42F8-9667-95CF6F1F5700}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA6B1F78-6D1D-4550-867C-D81A2584596E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="72e2bb9d-dac6-4618-b85f-5ec835598a0c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="97dd5345-e793-494f-a61a-0ff5f2d8588d"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Light modifications after eacher checkin
</commit_message>
<xml_diff>
--- a/UntitledKitchenGame/Game/UntitledKitchenGame/Assets/Editor/Items.xlsx
+++ b/UntitledKitchenGame/Game/UntitledKitchenGame/Assets/Editor/Items.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\placej\source\repos\UntitledKitchenGame\UntitledKitchenGame\Game\UntitledKitchenGame\Assets\Editor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D015D257-0390-4DDD-BBA0-2B2FB9878E41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D6CBC39-7678-4BF7-AB47-BCF22B51E1D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{F8B15126-9F65-4AA0-BFBE-7FC0EBE8032D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{F8B15126-9F65-4AA0-BFBE-7FC0EBE8032D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
   <si>
     <t>Points</t>
   </si>
@@ -160,6 +160,9 @@
   </si>
   <si>
     <t>Variables</t>
+  </si>
+  <si>
+    <t>Multiply string logic to have ands in filers or array values</t>
   </si>
 </sst>
 </file>
@@ -586,10 +589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2334730F-D581-4249-91BD-F969B819BCBB}">
-  <dimension ref="B1:Z22"/>
+  <dimension ref="B1:Z32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="W14" sqref="W14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -712,23 +715,23 @@
       </c>
       <c r="S4" t="str" cm="1">
         <f t="array" aca="1" ref="S4" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Beef</v>
+        <v>Rice</v>
       </c>
       <c r="U4" t="str" cm="1">
         <f t="array" aca="1" ref="U4" ca="1">IF(INDEX(Food[Name],OrderIndex)= OR(OrderIndex2,OrderIndex3),"FirstConTrue", INDEX(Food[Name],OrderIndex))</f>
-        <v>Chicken</v>
+        <v>Pasta</v>
       </c>
       <c r="V4" t="str" cm="1">
         <f t="array" aca="1" ref="V4" ca="1">IF(INDEX(Food[Name],OrderIndex2)= OR(OrderIndex,OrderIndex3),"FirstConTrue", INDEX(Food[Name],OrderIndex2))</f>
-        <v>Tuna</v>
+        <v>Chicken</v>
       </c>
       <c r="W4" t="str" cm="1">
         <f t="array" aca="1" ref="W4" ca="1">IF(INDEX(Food[Name],OrderIndex3)= OR(OrderIndex2,OrderIndex),"FirstConTrue", INDEX(Food[Name],OrderIndex3))</f>
-        <v>Tuna</v>
+        <v>Chicken</v>
       </c>
       <c r="X4" t="str">
         <f ca="1">_xlfn.CONCAT(J4:S4)</f>
-        <v>00000000Beef</v>
+        <v>00000000Rice</v>
       </c>
       <c r="Y4" t="e">
         <f ca="1">IF((U4+V4+W4) = X4, TRUE,FALSE)</f>
@@ -784,15 +787,15 @@
       </c>
       <c r="R5" t="str">
         <f ca="1">S4</f>
-        <v>Beef</v>
+        <v>Rice</v>
       </c>
       <c r="S5" t="str" cm="1">
         <f t="array" aca="1" ref="S5" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Beef</v>
+        <v>Lettuce</v>
       </c>
       <c r="U5" t="str" cm="1">
         <f t="array" aca="1" ref="U5" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Tuna</v>
+        <v>Carrot</v>
       </c>
       <c r="V5" t="str" cm="1">
         <f t="array" aca="1" ref="V5" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
@@ -800,11 +803,11 @@
       </c>
       <c r="W5" t="str" cm="1">
         <f t="array" aca="1" ref="W5" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Chicken</v>
+        <v>Carrot</v>
       </c>
       <c r="X5" t="str">
         <f t="shared" ref="X5:X6" ca="1" si="2">_xlfn.CONCAT(J5:S5)</f>
-        <v>0000000BeefBeef</v>
+        <v>0000000RiceLettuce</v>
       </c>
       <c r="Y5">
         <f ca="1">COUNTIF($J4:$S4, OR(U4,V4,W4))</f>
@@ -812,7 +815,7 @@
       </c>
       <c r="Z5">
         <f ca="1">COUNTIF($J5:$S5, U5) +COUNTIF($J5:$S5, V5) + COUNTIF($J5:$S5,W5)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:26">
@@ -860,31 +863,31 @@
       </c>
       <c r="Q6" t="str">
         <f ca="1">R5</f>
-        <v>Beef</v>
+        <v>Rice</v>
       </c>
       <c r="R6" t="str">
         <f ca="1">S5</f>
-        <v>Beef</v>
+        <v>Lettuce</v>
       </c>
       <c r="S6" t="str" cm="1">
         <f t="array" aca="1" ref="S6" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Salmon</v>
+        <v>Beef</v>
       </c>
       <c r="U6" t="str" cm="1">
         <f t="array" aca="1" ref="U6" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Onion</v>
+        <v>Tuna</v>
       </c>
       <c r="V6" t="str" cm="1">
         <f t="array" aca="1" ref="V6" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Onion</v>
+        <v>Salmon</v>
       </c>
       <c r="W6" t="str" cm="1">
         <f t="array" aca="1" ref="W6" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Bread</v>
+        <v>Tuna</v>
       </c>
       <c r="X6" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>000000BeefBeefSalmon</v>
+        <v>000000RiceLettuceBeef</v>
       </c>
       <c r="Z6">
         <f t="shared" ref="Z6:Z7" ca="1" si="3">COUNTIF($J6:$S6, U6) +COUNTIF($J6:$S6, V6) + COUNTIF($J6:$S6,W6)</f>
@@ -932,26 +935,26 @@
       </c>
       <c r="P7" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Beef</v>
+        <v>Rice</v>
       </c>
       <c r="Q7" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Beef</v>
+        <v>Lettuce</v>
       </c>
       <c r="R7" t="str">
         <f ca="1">S6</f>
-        <v>Salmon</v>
+        <v>Beef</v>
       </c>
       <c r="S7" t="str" cm="1">
         <f t="array" aca="1" ref="S7" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Beef</v>
+        <v>Salmon</v>
       </c>
       <c r="X7" t="str">
         <f ca="1">_xlfn.CONCAT(J7:S7)</f>
-        <v>00000BeefBeefSalmonBeef</v>
+        <v>00000RiceLettuceBeefSalmon</v>
       </c>
       <c r="Z7">
-        <f t="shared" ca="1" si="3"/>
+        <f ca="1">COUNTIF($J7:$S7, U7) +COUNTIF($J7:$S7, V7) + COUNTIF($J7:$S7,W7)</f>
         <v>15</v>
       </c>
     </row>
@@ -989,23 +992,23 @@
       </c>
       <c r="O8" t="str">
         <f t="shared" ca="1" si="1"/>
+        <v>Rice</v>
+      </c>
+      <c r="P8" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Lettuce</v>
+      </c>
+      <c r="Q8" t="str">
+        <f t="shared" ca="1" si="1"/>
         <v>Beef</v>
       </c>
-      <c r="P8" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Beef</v>
-      </c>
-      <c r="Q8" t="str">
+      <c r="R8" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>Salmon</v>
-      </c>
-      <c r="R8" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Beef</v>
       </c>
       <c r="S8" t="str" cm="1">
         <f t="array" aca="1" ref="S8" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Beef</v>
+        <v>Lobster</v>
       </c>
     </row>
     <row r="9" spans="2:26">
@@ -1038,27 +1041,27 @@
       </c>
       <c r="N9" t="str">
         <f t="shared" ca="1" si="0"/>
+        <v>Rice</v>
+      </c>
+      <c r="O9" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Lettuce</v>
+      </c>
+      <c r="P9" t="str">
+        <f t="shared" ca="1" si="1"/>
         <v>Beef</v>
       </c>
-      <c r="O9" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Beef</v>
-      </c>
-      <c r="P9" t="str">
+      <c r="Q9" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>Salmon</v>
       </c>
-      <c r="Q9" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Beef</v>
-      </c>
       <c r="R9" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Beef</v>
+        <v>Lobster</v>
       </c>
       <c r="S9" t="str" cm="1">
         <f t="array" aca="1" ref="S9" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Pasta</v>
+        <v>Lettuce</v>
       </c>
     </row>
     <row r="10" spans="2:26">
@@ -1087,31 +1090,31 @@
       </c>
       <c r="M10" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Beef</v>
+        <v>Rice</v>
       </c>
       <c r="N10" t="str">
         <f t="shared" ca="1" si="0"/>
+        <v>Lettuce</v>
+      </c>
+      <c r="O10" t="str">
+        <f t="shared" ca="1" si="1"/>
         <v>Beef</v>
       </c>
-      <c r="O10" t="str">
+      <c r="P10" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>Salmon</v>
       </c>
-      <c r="P10" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Beef</v>
-      </c>
       <c r="Q10" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Beef</v>
+        <v>Lobster</v>
       </c>
       <c r="R10" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Pasta</v>
+        <v>Lettuce</v>
       </c>
       <c r="S10" t="str" cm="1">
         <f t="array" aca="1" ref="S10" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Onion</v>
+        <v>Rice</v>
       </c>
     </row>
     <row r="11" spans="2:26">
@@ -1136,35 +1139,35 @@
       </c>
       <c r="L11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Beef</v>
+        <v>Rice</v>
       </c>
       <c r="M11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Beef</v>
+        <v>Lettuce</v>
       </c>
       <c r="N11" t="str">
         <f t="shared" ca="1" si="0"/>
+        <v>Beef</v>
+      </c>
+      <c r="O11" t="str">
+        <f t="shared" ca="1" si="1"/>
         <v>Salmon</v>
       </c>
-      <c r="O11" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Beef</v>
-      </c>
       <c r="P11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Beef</v>
+        <v>Lobster</v>
       </c>
       <c r="Q11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Pasta</v>
+        <v>Lettuce</v>
       </c>
       <c r="R11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Onion</v>
+        <v>Rice</v>
       </c>
       <c r="S11" t="str" cm="1">
         <f t="array" aca="1" ref="S11" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Pasta</v>
+        <v>Rice</v>
       </c>
     </row>
     <row r="12" spans="2:26">
@@ -1185,39 +1188,55 @@
       </c>
       <c r="K12" t="str">
         <f ca="1">L11</f>
-        <v>Beef</v>
+        <v>Rice</v>
       </c>
       <c r="L12" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Beef</v>
+        <v>Lettuce</v>
       </c>
       <c r="M12" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Salmon</v>
+        <v>Beef</v>
       </c>
       <c r="N12" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Beef</v>
+        <v>Salmon</v>
       </c>
       <c r="O12" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Beef</v>
+        <v>Lobster</v>
       </c>
       <c r="P12" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Pasta</v>
+        <v>Lettuce</v>
       </c>
       <c r="Q12" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Onion</v>
+        <v>Rice</v>
       </c>
       <c r="R12" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Pasta</v>
+        <v>Rice</v>
       </c>
       <c r="S12" t="str" cm="1">
         <f t="array" aca="1" ref="S12" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Lobster</v>
+        <v>Bread</v>
+      </c>
+      <c r="U12">
+        <f ca="1">COUNTIF($K$12:$S$12,U6)</f>
+        <v>0</v>
+      </c>
+      <c r="V12">
+        <f ca="1">MAX(0,COUNTIF($K$12:$S$12,V6)-(U6=V6))</f>
+        <v>1</v>
+      </c>
+      <c r="W12">
+        <f ca="1">MAX(0, COUNTIF($K$12:$S$12,W6)-(W6=V6)-(W6=U6))</f>
+        <v>0</v>
+      </c>
+      <c r="X12">
+        <f ca="1">SUM(U12:W12)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="2:26">
@@ -1270,9 +1289,9 @@
       <c r="F15">
         <v>1</v>
       </c>
-      <c r="U15" t="e" cm="1">
-        <f t="array" aca="1" ref="U15" ca="1">_xlfn.SINGLE(INDEX(_xlfn._xlws.FILTER(Food[],Food[Type]=OrderIncludes,"ERR"),RANDBETWEEN(0,COUNTA(Food[Type]))))</f>
-        <v>#REF!</v>
+      <c r="U15" t="str">
+        <f ca="1">INDEX(Food[Name],RANDBETWEEN(0,COUNTA(_xlfn.ANCHORARRAY(U17))))</f>
+        <v>Salmon</v>
       </c>
       <c r="V15" t="e" cm="1">
         <f t="array" aca="1" ref="V15" ca="1">_xlfn.SINGLE(INDEX(_xlfn._xlws.FILTER(Food[],Food[Points] = OR(OrderIncludes,OrderIncludes2,OrderIncludes3), "ERR"),RANDBETWEEN(0,3)))</f>
@@ -1283,83 +1302,105 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="17" spans="14:25">
-      <c r="U17" t="str" cm="1">
-        <f t="array" ref="U17:Y19">_xlfn._xlws.FILTER(Food[],Food[Type]=OrderIncludes,"ERR")</f>
+    <row r="16" spans="2:26">
+      <c r="U16" t="str" cm="1">
+        <f t="array" ref="U16:U24">_xlfn._xlws.FILTER(Food[Name],COUNTIF(U2:W2, Food[Type])&gt;0,"-")</f>
         <v>Bread</v>
       </c>
-      <c r="V17" t="str">
-        <v>Grain</v>
-      </c>
-      <c r="W17">
-        <v>10</v>
-      </c>
-      <c r="X17">
-        <v>100</v>
-      </c>
-      <c r="Y17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="14:25">
+      <c r="V16" t="str" cm="1">
+        <f t="array" aca="1" ref="V16" ca="1">INDEX(_xlfn.ANCHORARRAY(U16), RANDBETWEEN(1, ROWS(_xlfn.ANCHORARRAY(U16))))</f>
+        <v>Chicken</v>
+      </c>
+    </row>
+    <row r="17" spans="9:23">
+      <c r="U17" t="str">
+        <v>Pasta</v>
+      </c>
+    </row>
+    <row r="18" spans="9:23">
       <c r="U18" t="str">
-        <v>Pasta</v>
-      </c>
-      <c r="V18" t="str">
-        <v>Grain</v>
-      </c>
-      <c r="W18">
-        <v>10</v>
-      </c>
-      <c r="X18">
-        <v>100</v>
-      </c>
-      <c r="Y18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="14:25">
+        <v>Rice</v>
+      </c>
+    </row>
+    <row r="19" spans="9:23">
+      <c r="I19" t="s">
+        <v>31</v>
+      </c>
       <c r="U19" t="str">
-        <v>Rice</v>
-      </c>
-      <c r="V19" t="str">
-        <v>Grain</v>
-      </c>
-      <c r="W19">
-        <v>10</v>
-      </c>
-      <c r="X19">
-        <v>100</v>
-      </c>
-      <c r="Y19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="14:25">
+        <v>Beef</v>
+      </c>
+    </row>
+    <row r="20" spans="9:23">
+      <c r="U20" t="str">
+        <v>Pork</v>
+      </c>
+    </row>
+    <row r="21" spans="9:23">
       <c r="N21" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="22" spans="14:25">
+      <c r="U21" t="str">
+        <v>Chicken</v>
+      </c>
+    </row>
+    <row r="22" spans="9:23">
       <c r="N22">
         <f ca="1">RANDBETWEEN(1,COUNTA(Food[Name]))</f>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="O22">
         <f ca="1">RANDBETWEEN(1,COUNTA(Food[Type]))</f>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="P22">
         <f ca="1">RANDBETWEEN(1,COUNTA(Food[Points]))</f>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="R22" t="str" cm="1">
         <f t="array" aca="1" ref="R22" ca="1">IF(INDEX(Food[Name],OrderIndex2)= OR(OrderIndex,OrderIndex3), "-",INDEX(Food[Name],OrderIndex2))</f>
-        <v>Tuna</v>
+        <v>Chicken</v>
+      </c>
+      <c r="U22" t="str">
+        <v>Carrot</v>
+      </c>
+    </row>
+    <row r="23" spans="9:23">
+      <c r="U23" t="str">
+        <v>Onion</v>
+      </c>
+    </row>
+    <row r="24" spans="9:23">
+      <c r="U24" t="str">
+        <v>Lettuce</v>
+      </c>
+    </row>
+    <row r="30" spans="9:23">
+      <c r="V30" t="str" cm="1">
+        <f t="array" ref="V30:W32">_xlfn._xlws.FILTER(Food[[Name]:[Type]],Food[Type]=OrderIncludes,"-")</f>
+        <v>Bread</v>
+      </c>
+      <c r="W30" t="str">
+        <v>Grain</v>
+      </c>
+    </row>
+    <row r="31" spans="9:23">
+      <c r="V31" t="str">
+        <v>Pasta</v>
+      </c>
+      <c r="W31" t="str">
+        <v>Grain</v>
+      </c>
+    </row>
+    <row r="32" spans="9:23">
+      <c r="V32" t="str">
+        <v>Rice</v>
+      </c>
+      <c r="W32" t="str">
+        <v>Grain</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="3">
+  <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C15 U2:W2" xr:uid="{22784EBF-D91C-4A9F-BBF6-DF997D832606}">
       <formula1>INDIRECT("ItemTypes[Type]")</formula1>
     </dataValidation>

</xml_diff>

<commit_message>
Rarirty now operates with the item generator
</commit_message>
<xml_diff>
--- a/UntitledKitchenGame/Game/UntitledKitchenGame/Assets/Editor/Items.xlsx
+++ b/UntitledKitchenGame/Game/UntitledKitchenGame/Assets/Editor/Items.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\placej\source\repos\UntitledKitchenGame\UntitledKitchenGame\Game\UntitledKitchenGame\Assets\Editor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\murra\OneDrive\Documents\GitHub\UntitledKitchenGame\UntitledKitchenGame\Game\UntitledKitchenGame\Assets\Editor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D6CBC39-7678-4BF7-AB47-BCF22B51E1D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D51A9865-3D45-4F6B-8A9C-A9AD62CB3773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{F8B15126-9F65-4AA0-BFBE-7FC0EBE8032D}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F8B15126-9F65-4AA0-BFBE-7FC0EBE8032D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -169,7 +169,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -591,18 +591,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2334730F-D581-4249-91BD-F969B819BCBB}">
   <dimension ref="B1:Z32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="W14" sqref="W14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="18" width="9.375" customWidth="1"/>
-    <col min="24" max="24" width="42.125" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="18" width="9.42578125" customWidth="1"/>
+    <col min="24" max="24" width="42.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:26" ht="15" thickBot="1">
+    <row r="1" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J1" t="s">
         <v>25</v>
       </c>
@@ -610,7 +610,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="2:26" ht="15" thickBot="1">
+    <row r="2" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J2" t="s">
         <v>27</v>
       </c>
@@ -630,7 +630,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="2:26" s="1" customFormat="1">
+    <row r="3" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
@@ -662,7 +662,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="2:26">
+    <row r="4" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>9</v>
       </c>
@@ -673,7 +673,7 @@
         <v>10</v>
       </c>
       <c r="E4">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -715,15 +715,15 @@
       </c>
       <c r="S4" t="str" cm="1">
         <f t="array" aca="1" ref="S4" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Rice</v>
+        <v>Beef</v>
       </c>
       <c r="U4" t="str" cm="1">
         <f t="array" aca="1" ref="U4" ca="1">IF(INDEX(Food[Name],OrderIndex)= OR(OrderIndex2,OrderIndex3),"FirstConTrue", INDEX(Food[Name],OrderIndex))</f>
-        <v>Pasta</v>
+        <v>Pork</v>
       </c>
       <c r="V4" t="str" cm="1">
         <f t="array" aca="1" ref="V4" ca="1">IF(INDEX(Food[Name],OrderIndex2)= OR(OrderIndex,OrderIndex3),"FirstConTrue", INDEX(Food[Name],OrderIndex2))</f>
-        <v>Chicken</v>
+        <v>Rice</v>
       </c>
       <c r="W4" t="str" cm="1">
         <f t="array" aca="1" ref="W4" ca="1">IF(INDEX(Food[Name],OrderIndex3)= OR(OrderIndex2,OrderIndex),"FirstConTrue", INDEX(Food[Name],OrderIndex3))</f>
@@ -731,14 +731,14 @@
       </c>
       <c r="X4" t="str">
         <f ca="1">_xlfn.CONCAT(J4:S4)</f>
-        <v>00000000Rice</v>
+        <v>00000000Beef</v>
       </c>
       <c r="Y4" t="e">
         <f ca="1">IF((U4+V4+W4) = X4, TRUE,FALSE)</f>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="5" spans="2:26">
+    <row r="5" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>19</v>
       </c>
@@ -749,7 +749,7 @@
         <v>10</v>
       </c>
       <c r="E5">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -787,27 +787,27 @@
       </c>
       <c r="R5" t="str">
         <f ca="1">S4</f>
-        <v>Rice</v>
+        <v>Beef</v>
       </c>
       <c r="S5" t="str" cm="1">
         <f t="array" aca="1" ref="S5" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Lettuce</v>
+        <v>Pasta</v>
       </c>
       <c r="U5" t="str" cm="1">
         <f t="array" aca="1" ref="U5" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Carrot</v>
+        <v>Bread</v>
       </c>
       <c r="V5" t="str" cm="1">
         <f t="array" aca="1" ref="V5" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Lettuce</v>
+        <v>Carrot</v>
       </c>
       <c r="W5" t="str" cm="1">
         <f t="array" aca="1" ref="W5" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Carrot</v>
+        <v>Bread</v>
       </c>
       <c r="X5" t="str">
         <f t="shared" ref="X5:X6" ca="1" si="2">_xlfn.CONCAT(J5:S5)</f>
-        <v>0000000RiceLettuce</v>
+        <v>0000000BeefPasta</v>
       </c>
       <c r="Y5">
         <f ca="1">COUNTIF($J4:$S4, OR(U4,V4,W4))</f>
@@ -815,10 +815,10 @@
       </c>
       <c r="Z5">
         <f ca="1">COUNTIF($J5:$S5, U5) +COUNTIF($J5:$S5, V5) + COUNTIF($J5:$S5,W5)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="2:26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>20</v>
       </c>
@@ -829,7 +829,7 @@
         <v>10</v>
       </c>
       <c r="E6">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -863,23 +863,23 @@
       </c>
       <c r="Q6" t="str">
         <f ca="1">R5</f>
-        <v>Rice</v>
+        <v>Beef</v>
       </c>
       <c r="R6" t="str">
         <f ca="1">S5</f>
-        <v>Lettuce</v>
+        <v>Pasta</v>
       </c>
       <c r="S6" t="str" cm="1">
         <f t="array" aca="1" ref="S6" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Beef</v>
+        <v>Pork</v>
       </c>
       <c r="U6" t="str" cm="1">
         <f t="array" aca="1" ref="U6" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Tuna</v>
+        <v>Carrot</v>
       </c>
       <c r="V6" t="str" cm="1">
         <f t="array" aca="1" ref="V6" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Salmon</v>
+        <v>Beef</v>
       </c>
       <c r="W6" t="str" cm="1">
         <f t="array" aca="1" ref="W6" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
@@ -887,14 +887,14 @@
       </c>
       <c r="X6" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>000000RiceLettuceBeef</v>
+        <v>000000BeefPastaPork</v>
       </c>
       <c r="Z6">
-        <f t="shared" ref="Z6:Z7" ca="1" si="3">COUNTIF($J6:$S6, U6) +COUNTIF($J6:$S6, V6) + COUNTIF($J6:$S6,W6)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="2:26">
+        <f t="shared" ref="Z6" ca="1" si="3">COUNTIF($J6:$S6, U6) +COUNTIF($J6:$S6, V6) + COUNTIF($J6:$S6,W6)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>11</v>
       </c>
@@ -905,7 +905,7 @@
         <v>10</v>
       </c>
       <c r="E7">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -935,30 +935,30 @@
       </c>
       <c r="P7" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Rice</v>
+        <v>Beef</v>
       </c>
       <c r="Q7" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Lettuce</v>
+        <v>Pasta</v>
       </c>
       <c r="R7" t="str">
         <f ca="1">S6</f>
-        <v>Beef</v>
+        <v>Pork</v>
       </c>
       <c r="S7" t="str" cm="1">
         <f t="array" aca="1" ref="S7" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Salmon</v>
+        <v>Rice</v>
       </c>
       <c r="X7" t="str">
         <f ca="1">_xlfn.CONCAT(J7:S7)</f>
-        <v>00000RiceLettuceBeefSalmon</v>
+        <v>00000BeefPastaPorkRice</v>
       </c>
       <c r="Z7">
         <f ca="1">COUNTIF($J7:$S7, U7) +COUNTIF($J7:$S7, V7) + COUNTIF($J7:$S7,W7)</f>
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="2:26">
+    <row r="8" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>21</v>
       </c>
@@ -969,7 +969,7 @@
         <v>10</v>
       </c>
       <c r="E8">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -992,26 +992,26 @@
       </c>
       <c r="O8" t="str">
         <f t="shared" ca="1" si="1"/>
+        <v>Beef</v>
+      </c>
+      <c r="P8" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Pasta</v>
+      </c>
+      <c r="Q8" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Pork</v>
+      </c>
+      <c r="R8" t="str">
+        <f t="shared" ca="1" si="1"/>
         <v>Rice</v>
-      </c>
-      <c r="P8" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Lettuce</v>
-      </c>
-      <c r="Q8" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Beef</v>
-      </c>
-      <c r="R8" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Salmon</v>
       </c>
       <c r="S8" t="str" cm="1">
         <f t="array" aca="1" ref="S8" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Lobster</v>
-      </c>
-    </row>
-    <row r="9" spans="2:26">
+        <v>Carrot</v>
+      </c>
+    </row>
+    <row r="9" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>22</v>
       </c>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E9">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="F9">
         <v>1</v>
@@ -1041,30 +1041,30 @@
       </c>
       <c r="N9" t="str">
         <f t="shared" ca="1" si="0"/>
+        <v>Beef</v>
+      </c>
+      <c r="O9" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Pasta</v>
+      </c>
+      <c r="P9" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Pork</v>
+      </c>
+      <c r="Q9" t="str">
+        <f t="shared" ca="1" si="1"/>
         <v>Rice</v>
       </c>
-      <c r="O9" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Lettuce</v>
-      </c>
-      <c r="P9" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Beef</v>
-      </c>
-      <c r="Q9" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Salmon</v>
-      </c>
       <c r="R9" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Lobster</v>
+        <v>Carrot</v>
       </c>
       <c r="S9" t="str" cm="1">
         <f t="array" aca="1" ref="S9" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Lettuce</v>
-      </c>
-    </row>
-    <row r="10" spans="2:26">
+        <v>Lobster</v>
+      </c>
+    </row>
+    <row r="10" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>7</v>
       </c>
@@ -1075,7 +1075,7 @@
         <v>10</v>
       </c>
       <c r="E10">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -1090,34 +1090,34 @@
       </c>
       <c r="M10" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Rice</v>
+        <v>Beef</v>
       </c>
       <c r="N10" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Lettuce</v>
+        <v>Pasta</v>
       </c>
       <c r="O10" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Beef</v>
+        <v>Pork</v>
       </c>
       <c r="P10" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Salmon</v>
+        <v>Rice</v>
       </c>
       <c r="Q10" t="str">
         <f t="shared" ca="1" si="1"/>
+        <v>Carrot</v>
+      </c>
+      <c r="R10" t="str">
+        <f t="shared" ca="1" si="1"/>
         <v>Lobster</v>
-      </c>
-      <c r="R10" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Lettuce</v>
       </c>
       <c r="S10" t="str" cm="1">
         <f t="array" aca="1" ref="S10" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Rice</v>
-      </c>
-    </row>
-    <row r="11" spans="2:26">
+        <v>Pasta</v>
+      </c>
+    </row>
+    <row r="11" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>17</v>
       </c>
@@ -1128,7 +1128,7 @@
         <v>10</v>
       </c>
       <c r="E11">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="F11">
         <v>1</v>
@@ -1139,38 +1139,38 @@
       </c>
       <c r="L11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Rice</v>
+        <v>Beef</v>
       </c>
       <c r="M11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Lettuce</v>
+        <v>Pasta</v>
       </c>
       <c r="N11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Beef</v>
+        <v>Pork</v>
       </c>
       <c r="O11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Salmon</v>
+        <v>Rice</v>
       </c>
       <c r="P11" t="str">
         <f t="shared" ca="1" si="1"/>
+        <v>Carrot</v>
+      </c>
+      <c r="Q11" t="str">
+        <f t="shared" ca="1" si="1"/>
         <v>Lobster</v>
       </c>
-      <c r="Q11" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Lettuce</v>
-      </c>
       <c r="R11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Rice</v>
+        <v>Pasta</v>
       </c>
       <c r="S11" t="str" cm="1">
         <f t="array" aca="1" ref="S11" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Rice</v>
-      </c>
-    </row>
-    <row r="12" spans="2:26">
+        <v>Bread</v>
+      </c>
+    </row>
+    <row r="12" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>18</v>
       </c>
@@ -1181,50 +1181,50 @@
         <v>10</v>
       </c>
       <c r="E12">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="F12">
         <v>1</v>
       </c>
       <c r="K12" t="str">
         <f ca="1">L11</f>
-        <v>Rice</v>
+        <v>Beef</v>
       </c>
       <c r="L12" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Lettuce</v>
+        <v>Pasta</v>
       </c>
       <c r="M12" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Beef</v>
+        <v>Pork</v>
       </c>
       <c r="N12" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Salmon</v>
+        <v>Rice</v>
       </c>
       <c r="O12" t="str">
         <f t="shared" ca="1" si="1"/>
+        <v>Carrot</v>
+      </c>
+      <c r="P12" t="str">
+        <f t="shared" ca="1" si="1"/>
         <v>Lobster</v>
       </c>
-      <c r="P12" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Lettuce</v>
-      </c>
       <c r="Q12" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Rice</v>
+        <v>Pasta</v>
       </c>
       <c r="R12" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Rice</v>
+        <v>Bread</v>
       </c>
       <c r="S12" t="str" cm="1">
         <f t="array" aca="1" ref="S12" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Bread</v>
+        <v>Chicken</v>
       </c>
       <c r="U12">
         <f ca="1">COUNTIF($K$12:$S$12,U6)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V12">
         <f ca="1">MAX(0,COUNTIF($K$12:$S$12,V6)-(U6=V6))</f>
@@ -1236,10 +1236,10 @@
       </c>
       <c r="X12">
         <f ca="1">SUM(U12:W12)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="2:26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>8</v>
       </c>
@@ -1250,13 +1250,13 @@
         <v>10</v>
       </c>
       <c r="E13">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:26">
+    <row r="14" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>23</v>
       </c>
@@ -1267,13 +1267,13 @@
         <v>10</v>
       </c>
       <c r="E14">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="F14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:26">
+    <row r="15" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>24</v>
       </c>
@@ -1284,14 +1284,14 @@
         <v>10</v>
       </c>
       <c r="E15">
-        <v>100</v>
+        <v>15</v>
       </c>
       <c r="F15">
         <v>1</v>
       </c>
       <c r="U15" t="str">
         <f ca="1">INDEX(Food[Name],RANDBETWEEN(0,COUNTA(_xlfn.ANCHORARRAY(U17))))</f>
-        <v>Salmon</v>
+        <v>Lettuce</v>
       </c>
       <c r="V15" t="e" cm="1">
         <f t="array" aca="1" ref="V15" ca="1">_xlfn.SINGLE(INDEX(_xlfn._xlws.FILTER(Food[],Food[Points] = OR(OrderIncludes,OrderIncludes2,OrderIncludes3), "ERR"),RANDBETWEEN(0,3)))</f>
@@ -1302,27 +1302,27 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="16" spans="2:26">
+    <row r="16" spans="2:26" x14ac:dyDescent="0.25">
       <c r="U16" t="str" cm="1">
         <f t="array" ref="U16:U24">_xlfn._xlws.FILTER(Food[Name],COUNTIF(U2:W2, Food[Type])&gt;0,"-")</f>
         <v>Bread</v>
       </c>
       <c r="V16" t="str" cm="1">
         <f t="array" aca="1" ref="V16" ca="1">INDEX(_xlfn.ANCHORARRAY(U16), RANDBETWEEN(1, ROWS(_xlfn.ANCHORARRAY(U16))))</f>
-        <v>Chicken</v>
-      </c>
-    </row>
-    <row r="17" spans="9:23">
+        <v>Pasta</v>
+      </c>
+    </row>
+    <row r="17" spans="9:23" x14ac:dyDescent="0.25">
       <c r="U17" t="str">
         <v>Pasta</v>
       </c>
     </row>
-    <row r="18" spans="9:23">
+    <row r="18" spans="9:23" x14ac:dyDescent="0.25">
       <c r="U18" t="str">
         <v>Rice</v>
       </c>
     </row>
-    <row r="19" spans="9:23">
+    <row r="19" spans="9:23" x14ac:dyDescent="0.25">
       <c r="I19" t="s">
         <v>31</v>
       </c>
@@ -1330,12 +1330,12 @@
         <v>Beef</v>
       </c>
     </row>
-    <row r="20" spans="9:23">
+    <row r="20" spans="9:23" x14ac:dyDescent="0.25">
       <c r="U20" t="str">
         <v>Pork</v>
       </c>
     </row>
-    <row r="21" spans="9:23">
+    <row r="21" spans="9:23" x14ac:dyDescent="0.25">
       <c r="N21" t="s">
         <v>30</v>
       </c>
@@ -1343,14 +1343,14 @@
         <v>Chicken</v>
       </c>
     </row>
-    <row r="22" spans="9:23">
+    <row r="22" spans="9:23" x14ac:dyDescent="0.25">
       <c r="N22">
         <f ca="1">RANDBETWEEN(1,COUNTA(Food[Name]))</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="O22">
         <f ca="1">RANDBETWEEN(1,COUNTA(Food[Type]))</f>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="P22">
         <f ca="1">RANDBETWEEN(1,COUNTA(Food[Points]))</f>
@@ -1358,23 +1358,23 @@
       </c>
       <c r="R22" t="str" cm="1">
         <f t="array" aca="1" ref="R22" ca="1">IF(INDEX(Food[Name],OrderIndex2)= OR(OrderIndex,OrderIndex3), "-",INDEX(Food[Name],OrderIndex2))</f>
-        <v>Chicken</v>
+        <v>Rice</v>
       </c>
       <c r="U22" t="str">
         <v>Carrot</v>
       </c>
     </row>
-    <row r="23" spans="9:23">
+    <row r="23" spans="9:23" x14ac:dyDescent="0.25">
       <c r="U23" t="str">
         <v>Onion</v>
       </c>
     </row>
-    <row r="24" spans="9:23">
+    <row r="24" spans="9:23" x14ac:dyDescent="0.25">
       <c r="U24" t="str">
         <v>Lettuce</v>
       </c>
     </row>
-    <row r="30" spans="9:23">
+    <row r="30" spans="9:23" x14ac:dyDescent="0.25">
       <c r="V30" t="str" cm="1">
         <f t="array" ref="V30:W32">_xlfn._xlws.FILTER(Food[[Name]:[Type]],Food[Type]=OrderIncludes,"-")</f>
         <v>Bread</v>
@@ -1383,7 +1383,7 @@
         <v>Grain</v>
       </c>
     </row>
-    <row r="31" spans="9:23">
+    <row r="31" spans="9:23" x14ac:dyDescent="0.25">
       <c r="V31" t="str">
         <v>Pasta</v>
       </c>
@@ -1391,7 +1391,7 @@
         <v>Grain</v>
       </c>
     </row>
-    <row r="32" spans="9:23">
+    <row r="32" spans="9:23" x14ac:dyDescent="0.25">
       <c r="V32" t="str">
         <v>Rice</v>
       </c>
@@ -1422,6 +1422,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="97dd5345-e793-494f-a61a-0ff5f2d8588d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EB9F34A24037AB4FA470085E68A4B53B" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1f05ce8c82e9282909648c3323760eae">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="97dd5345-e793-494f-a61a-0ff5f2d8588d" xmlns:ns4="72e2bb9d-dac6-4618-b85f-5ec835598a0c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c14bf05b446930f087596548c801372f" ns3:_="" ns4:_="">
     <xsd:import namespace="97dd5345-e793-494f-a61a-0ff5f2d8588d"/>
@@ -1648,24 +1665,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA6B1F78-6D1D-4550-867C-D81A2584596E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="72e2bb9d-dac6-4618-b85f-5ec835598a0c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="97dd5345-e793-494f-a61a-0ff5f2d8588d"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="97dd5345-e793-494f-a61a-0ff5f2d8588d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB2BC082-80AE-42F8-9667-95CF6F1F5700}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{65537B17-CCB8-447E-A12B-556BEEDE4DB0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1682,29 +1707,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB2BC082-80AE-42F8-9667-95CF6F1F5700}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA6B1F78-6D1D-4550-867C-D81A2584596E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="72e2bb9d-dac6-4618-b85f-5ec835598a0c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="97dd5345-e793-494f-a61a-0ff5f2d8588d"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Tried making binomial distribution calc
</commit_message>
<xml_diff>
--- a/UntitledKitchenGame/Game/UntitledKitchenGame/Assets/Editor/Items.xlsx
+++ b/UntitledKitchenGame/Game/UntitledKitchenGame/Assets/Editor/Items.xlsx
@@ -1,28 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\murra\OneDrive\Documents\GitHub\UntitledKitchenGame\UntitledKitchenGame\Game\UntitledKitchenGame\Assets\Editor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D51A9865-3D45-4F6B-8A9C-A9AD62CB3773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF09E6A1-EC52-4582-B53A-66D846B25D84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F8B15126-9F65-4AA0-BFBE-7FC0EBE8032D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F8B15126-9F65-4AA0-BFBE-7FC0EBE8032D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Vairables" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="AvailableItems">Sheet1!$L$16</definedName>
     <definedName name="ItemType">ItemTypes[[#Headers],[Type]]</definedName>
-    <definedName name="OrderIncludes">Sheet1!$U$2</definedName>
-    <definedName name="OrderIncludes2">Sheet1!$V$2</definedName>
-    <definedName name="OrderIncludes3">Sheet1!$W$2</definedName>
-    <definedName name="OrderIndex">Sheet1!$N$22</definedName>
-    <definedName name="OrderIndex2">Sheet1!$O$22</definedName>
-    <definedName name="OrderIndex3">Sheet1!$P$22</definedName>
+    <definedName name="OrderIncludes">Sheet1!$AA$3</definedName>
+    <definedName name="OrderIncludes2">Sheet1!$AB$3</definedName>
+    <definedName name="OrderIncludes3">Sheet1!$AC$3</definedName>
+    <definedName name="OrderIndex">Sheet1!$E$30</definedName>
+    <definedName name="OrderIndex2">Sheet1!$F$30</definedName>
+    <definedName name="OrderIndex3">Sheet1!$G$30</definedName>
+    <definedName name="OrderMax">Sheet1!$K$5</definedName>
+    <definedName name="testFilter">Sheet1!$L$16</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -67,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="32">
   <si>
     <t>Points</t>
   </si>
@@ -144,32 +148,32 @@
     <t>Lettuce</t>
   </si>
   <si>
-    <t>Items</t>
-  </si>
-  <si>
     <t>New Item</t>
   </si>
   <si>
-    <t>Final Slot</t>
-  </si>
-  <si>
-    <t>Experiements?</t>
-  </si>
-  <si>
     <t>Order Includes…</t>
   </si>
   <si>
     <t>Variables</t>
   </si>
   <si>
-    <t>Multiply string logic to have ands in filers or array values</t>
+    <t>Order 2</t>
+  </si>
+  <si>
+    <t>Order 3</t>
+  </si>
+  <si>
+    <t>Order Max</t>
+  </si>
+  <si>
+    <t>AvailableItems</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -177,16 +181,44 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="2"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -209,16 +241,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -244,8 +293,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{35FB6A7E-F941-41ED-AF7A-CE78317F833A}" name="ItemTypes" displayName="ItemTypes" ref="H3:H7" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="H3:H7" xr:uid="{35FB6A7E-F941-41ED-AF7A-CE78317F833A}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{35FB6A7E-F941-41ED-AF7A-CE78317F833A}" name="ItemTypes" displayName="ItemTypes" ref="H4:H8" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="H4:H8" xr:uid="{35FB6A7E-F941-41ED-AF7A-CE78317F833A}">
     <filterColumn colId="0" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="1">
@@ -256,10 +305,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7AE9A713-C3CE-48AC-B440-488A7CD3381A}" name="Food" displayName="Food" ref="B3:F15" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="B3:F15" xr:uid="{7AE9A713-C3CE-48AC-B440-488A7CD3381A}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:F15">
-    <sortCondition ref="C3:C15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7AE9A713-C3CE-48AC-B440-488A7CD3381A}" name="Food" displayName="Food" ref="B4:F16" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="B4:F16" xr:uid="{7AE9A713-C3CE-48AC-B440-488A7CD3381A}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:F16">
+    <sortCondition ref="C4:C16"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{680C3E85-364D-401E-80B1-7407A04F49D6}" name="Name"/>
@@ -589,158 +638,114 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2334730F-D581-4249-91BD-F969B819BCBB}">
-  <dimension ref="B1:Z32"/>
+  <dimension ref="B2:AI39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="18" width="9.42578125" customWidth="1"/>
-    <col min="24" max="24" width="42.140625" customWidth="1"/>
+    <col min="9" max="10" width="9.42578125" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" customWidth="1"/>
+    <col min="12" max="24" width="9.42578125" customWidth="1"/>
+    <col min="30" max="30" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J1" t="s">
+    <row r="2" spans="2:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AA2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
+      <c r="AD2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AG2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AH2" s="2"/>
+      <c r="AI2" s="2"/>
+    </row>
+    <row r="3" spans="2:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Y3" t="s">
         <v>25</v>
       </c>
-      <c r="U1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J2" t="s">
-        <v>27</v>
-      </c>
-      <c r="S2" t="s">
-        <v>26</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="V2" s="2" t="s">
+      <c r="AA3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="AC3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="Y2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
+      <c r="AG3" s="2"/>
+      <c r="AH3" s="2"/>
+      <c r="AI3" s="2"/>
+    </row>
+    <row r="4" spans="2:35" s="1" customFormat="1" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="T3" s="1" t="s">
+      <c r="K4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="Z4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="U3" s="1" t="s">
+      <c r="AA4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="V3" s="1" t="s">
+      <c r="AB4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="W3" s="1" t="s">
+      <c r="AC4" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="AD4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="AI4" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="2:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
         <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4">
-        <v>10</v>
-      </c>
-      <c r="E4">
-        <v>10</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="H4" t="s">
-        <v>4</v>
-      </c>
-      <c r="K4">
-        <f>L3</f>
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <f t="shared" ref="K4:N12" si="0">M3</f>
-        <v>0</v>
-      </c>
-      <c r="M4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O4">
-        <f t="shared" ref="O4:R12" si="1">P3</f>
-        <v>0</v>
-      </c>
-      <c r="P4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R4">
-        <f>S3</f>
-        <v>0</v>
-      </c>
-      <c r="S4" t="str" cm="1">
-        <f t="array" aca="1" ref="S4" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Beef</v>
-      </c>
-      <c r="U4" t="str" cm="1">
-        <f t="array" aca="1" ref="U4" ca="1">IF(INDEX(Food[Name],OrderIndex)= OR(OrderIndex2,OrderIndex3),"FirstConTrue", INDEX(Food[Name],OrderIndex))</f>
-        <v>Pork</v>
-      </c>
-      <c r="V4" t="str" cm="1">
-        <f t="array" aca="1" ref="V4" ca="1">IF(INDEX(Food[Name],OrderIndex2)= OR(OrderIndex,OrderIndex3),"FirstConTrue", INDEX(Food[Name],OrderIndex2))</f>
-        <v>Rice</v>
-      </c>
-      <c r="W4" t="str" cm="1">
-        <f t="array" aca="1" ref="W4" ca="1">IF(INDEX(Food[Name],OrderIndex3)= OR(OrderIndex2,OrderIndex),"FirstConTrue", INDEX(Food[Name],OrderIndex3))</f>
-        <v>Chicken</v>
-      </c>
-      <c r="X4" t="str">
-        <f ca="1">_xlfn.CONCAT(J4:S4)</f>
-        <v>00000000Beef</v>
-      </c>
-      <c r="Y4" t="e">
-        <f ca="1">IF((U4+V4+W4) = X4, TRUE,FALSE)</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="5" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>19</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
@@ -749,78 +754,102 @@
         <v>10</v>
       </c>
       <c r="E5">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
       <c r="H5" t="s">
+        <v>4</v>
+      </c>
+      <c r="K5" s="6">
+        <v>3</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="N5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="K5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q5">
-        <f>R4</f>
-        <v>0</v>
-      </c>
-      <c r="R5" t="str">
-        <f ca="1">S4</f>
-        <v>Beef</v>
+      <c r="Q5" t="str" cm="1">
+        <f t="array" aca="1" ref="Q5" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
+        <v>Pork</v>
+      </c>
+      <c r="R5" t="str" cm="1">
+        <f t="array" aca="1" ref="R5" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
+        <v>Pork</v>
       </c>
       <c r="S5" t="str" cm="1">
         <f t="array" aca="1" ref="S5" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Pasta</v>
+        <v>Salmon</v>
+      </c>
+      <c r="T5" t="str" cm="1">
+        <f t="array" aca="1" ref="T5" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
+        <v>Carrot</v>
       </c>
       <c r="U5" t="str" cm="1">
         <f t="array" aca="1" ref="U5" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Bread</v>
+        <v>Pasta</v>
       </c>
       <c r="V5" t="str" cm="1">
         <f t="array" aca="1" ref="V5" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Carrot</v>
+        <v>Salmon</v>
       </c>
       <c r="W5" t="str" cm="1">
         <f t="array" aca="1" ref="W5" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
+        <v>Lettuce</v>
+      </c>
+      <c r="X5" t="str" cm="1">
+        <f t="array" aca="1" ref="X5" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
+        <v>Onion</v>
+      </c>
+      <c r="Y5" t="str" cm="1">
+        <f t="array" aca="1" ref="Y5" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
+        <v>Salmon</v>
+      </c>
+      <c r="AA5" s="2" t="str" cm="1">
+        <f t="array" aca="1" ref="AA5" ca="1">IF(INDEX(_xlfn.ANCHORARRAY(AvailableItems),OrderIndex)= OR(OrderIndex2,OrderIndex3),"FirstConTrue", INDEX(_xlfn.ANCHORARRAY(AvailableItems),OrderIndex))</f>
+        <v>Rice</v>
+      </c>
+      <c r="AB5" s="2" t="str" cm="1">
+        <f t="array" aca="1" ref="AB5" ca="1">IF(INDEX(_xlfn.ANCHORARRAY(AvailableItems),OrderIndex2)= OR(OrderIndex,OrderIndex3),"FirstConTrue", INDEX(_xlfn.ANCHORARRAY(AvailableItems),OrderIndex2))</f>
         <v>Bread</v>
       </c>
-      <c r="X5" t="str">
-        <f t="shared" ref="X5:X6" ca="1" si="2">_xlfn.CONCAT(J5:S5)</f>
-        <v>0000000BeefPasta</v>
-      </c>
-      <c r="Y5">
-        <f ca="1">COUNTIF($J4:$S4, OR(U4,V4,W4))</f>
-        <v>0</v>
-      </c>
-      <c r="Z5">
-        <f ca="1">COUNTIF($J5:$S5, U5) +COUNTIF($J5:$S5, V5) + COUNTIF($J5:$S5,W5)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="AC5" s="2" t="str" cm="1">
+        <f t="array" aca="1" ref="AC5" ca="1">IF(INDEX(_xlfn.ANCHORARRAY(AvailableItems),OrderIndex3)= OR(OrderIndex2,OrderIndex),"FirstConTrue", INDEX(_xlfn.ANCHORARRAY(AvailableItems),OrderIndex3))</f>
+        <v>Pork</v>
+      </c>
+      <c r="AD5" t="str" cm="1">
+        <f t="array" aca="1" ref="AD5" ca="1">IF(INDEX(_xlfn.ANCHORARRAY(AvailableItems),E31)= OR(F31,G31),"FirstConTrue", INDEX(_xlfn.ANCHORARRAY(AvailableItems),E31))</f>
+        <v>Chicken</v>
+      </c>
+      <c r="AE5" t="str" cm="1">
+        <f t="array" aca="1" ref="AE5" ca="1">IF(INDEX(_xlfn.ANCHORARRAY(AvailableItems),F31)= OR(G31,E31),"FirstConTrue", INDEX(_xlfn.ANCHORARRAY(AvailableItems),F31))</f>
+        <v>Chicken</v>
+      </c>
+      <c r="AF5" t="str" cm="1">
+        <f t="array" aca="1" ref="AF5" ca="1">IF(INDEX(_xlfn.ANCHORARRAY(AvailableItems),G31)= OR(E31,F31),"FirstConTrue", INDEX(_xlfn.ANCHORARRAY(AvailableItems),G31))</f>
+        <v>Chicken</v>
+      </c>
+      <c r="AG5" s="2" t="str" cm="1">
+        <f t="array" aca="1" ref="AG5" ca="1">IF(INDEX(_xlfn.ANCHORARRAY(AvailableItems),E32)= OR(F32,G32),"FirstConTrue", INDEX(_xlfn.ANCHORARRAY(AvailableItems),E32))</f>
+        <v>Pasta</v>
+      </c>
+      <c r="AH5" s="2" t="str" cm="1">
+        <f t="array" aca="1" ref="AH5" ca="1">IF(INDEX(_xlfn.ANCHORARRAY(AvailableItems),F32)= OR(G32,E32),"FirstConTrue", INDEX(_xlfn.ANCHORARRAY(AvailableItems),F32))</f>
+        <v>Chicken</v>
+      </c>
+      <c r="AI5" s="2" t="str" cm="1">
+        <f t="array" aca="1" ref="AI5" ca="1">IF(INDEX(_xlfn.ANCHORARRAY(AvailableItems),G32)= OR(F32,E32),"FirstConTrue", INDEX(_xlfn.ANCHORARRAY(AvailableItems),G32))</f>
+        <v>Rice</v>
+      </c>
+    </row>
+    <row r="6" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -829,138 +858,57 @@
         <v>10</v>
       </c>
       <c r="E6">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="H6" t="s">
+        <v>5</v>
+      </c>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1" t="str" cm="1">
+        <f t="array" ref="O6:O14">_xlfn._xlws.FILTER(Food[Name],COUNTIF(L5:N5, Food[Type])&gt;0,"-")</f>
+        <v>Bread</v>
+      </c>
+    </row>
+    <row r="7" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
         <v>6</v>
       </c>
-      <c r="K6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q6" t="str">
-        <f ca="1">R5</f>
-        <v>Beef</v>
-      </c>
-      <c r="R6" t="str">
-        <f ca="1">S5</f>
-        <v>Pasta</v>
-      </c>
-      <c r="S6" t="str" cm="1">
-        <f t="array" aca="1" ref="S6" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Pork</v>
-      </c>
-      <c r="U6" t="str" cm="1">
-        <f t="array" aca="1" ref="U6" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Carrot</v>
-      </c>
-      <c r="V6" t="str" cm="1">
-        <f t="array" aca="1" ref="V6" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Beef</v>
-      </c>
-      <c r="W6" t="str" cm="1">
-        <f t="array" aca="1" ref="W6" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Tuna</v>
-      </c>
-      <c r="X6" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>000000BeefPastaPork</v>
-      </c>
-      <c r="Z6">
-        <f t="shared" ref="Z6" ca="1" si="3">COUNTIF($J6:$S6, U6) +COUNTIF($J6:$S6, V6) + COUNTIF($J6:$S6,W6)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
       <c r="D7">
         <v>10</v>
       </c>
       <c r="E7">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="F7">
         <v>1</v>
       </c>
       <c r="H7" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="K7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P7" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Beef</v>
-      </c>
-      <c r="Q7" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f>_xlfn.BINOM.DIST(OrderMax,COUNTA(_xlfn.ANCHORARRAY(O6)),1/COUNTA(_xlfn.ANCHORARRAY(O6)),TRUE)</f>
+        <v>0.98789364751434194</v>
+      </c>
+      <c r="O7" t="str">
         <v>Pasta</v>
       </c>
-      <c r="R7" t="str">
-        <f ca="1">S6</f>
-        <v>Pork</v>
-      </c>
-      <c r="S7" t="str" cm="1">
-        <f t="array" aca="1" ref="S7" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Rice</v>
-      </c>
-      <c r="X7" t="str">
-        <f ca="1">_xlfn.CONCAT(J7:S7)</f>
-        <v>00000BeefPastaPorkRice</v>
-      </c>
-      <c r="Z7">
-        <f ca="1">COUNTIF($J7:$S7, U7) +COUNTIF($J7:$S7, V7) + COUNTIF($J7:$S7,W7)</f>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="AD7" t="str">
+        <f t="shared" ref="AD7" si="0">_xlfn.CONCAT(P7:Y7)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
@@ -969,51 +917,25 @@
         <v>10</v>
       </c>
       <c r="E8">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
-      <c r="K8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N8">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="H8" t="s">
+        <v>10</v>
       </c>
       <c r="O8" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Beef</v>
-      </c>
-      <c r="P8" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Pasta</v>
-      </c>
-      <c r="Q8" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Pork</v>
-      </c>
-      <c r="R8" t="str">
-        <f t="shared" ca="1" si="1"/>
         <v>Rice</v>
       </c>
-      <c r="S8" t="str" cm="1">
-        <f t="array" aca="1" ref="S8" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Carrot</v>
-      </c>
-    </row>
-    <row r="9" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="AD8" t="str">
+        <f>_xlfn.CONCAT(P8:Y8)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
@@ -1022,104 +944,38 @@
         <v>10</v>
       </c>
       <c r="E9">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="F9">
         <v>1</v>
       </c>
-      <c r="K9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N9" t="str">
-        <f t="shared" ca="1" si="0"/>
+      <c r="O9" t="str">
         <v>Beef</v>
       </c>
-      <c r="O9" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Pasta</v>
-      </c>
-      <c r="P9" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Pork</v>
-      </c>
-      <c r="Q9" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Rice</v>
-      </c>
-      <c r="R9" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Carrot</v>
-      </c>
-      <c r="S9" t="str" cm="1">
-        <f t="array" aca="1" ref="S9" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Lobster</v>
-      </c>
-    </row>
-    <row r="10" spans="2:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D10">
         <v>10</v>
       </c>
       <c r="E10">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="F10">
         <v>1</v>
       </c>
-      <c r="K10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M10" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Beef</v>
-      </c>
-      <c r="N10" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Pasta</v>
-      </c>
       <c r="O10" t="str">
-        <f t="shared" ca="1" si="1"/>
         <v>Pork</v>
       </c>
-      <c r="P10" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Rice</v>
-      </c>
-      <c r="Q10" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Carrot</v>
-      </c>
-      <c r="R10" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Lobster</v>
-      </c>
-      <c r="S10" t="str" cm="1">
-        <f t="array" aca="1" ref="S10" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Pasta</v>
-      </c>
-    </row>
-    <row r="11" spans="2:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -1128,51 +984,18 @@
         <v>10</v>
       </c>
       <c r="E11">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="F11">
         <v>1</v>
       </c>
-      <c r="K11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L11" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Beef</v>
-      </c>
-      <c r="M11" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Pasta</v>
-      </c>
-      <c r="N11" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Pork</v>
-      </c>
       <c r="O11" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Rice</v>
-      </c>
-      <c r="P11" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Carrot</v>
-      </c>
-      <c r="Q11" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Lobster</v>
-      </c>
-      <c r="R11" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Pasta</v>
-      </c>
-      <c r="S11" t="str" cm="1">
-        <f t="array" aca="1" ref="S11" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Bread</v>
-      </c>
-    </row>
-    <row r="12" spans="2:26" x14ac:dyDescent="0.25">
+        <v>Chicken</v>
+      </c>
+    </row>
+    <row r="12" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
@@ -1181,84 +1004,38 @@
         <v>10</v>
       </c>
       <c r="E12">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="F12">
         <v>1</v>
       </c>
-      <c r="K12" t="str">
-        <f ca="1">L11</f>
-        <v>Beef</v>
-      </c>
-      <c r="L12" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Pasta</v>
-      </c>
-      <c r="M12" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Pork</v>
-      </c>
-      <c r="N12" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Rice</v>
-      </c>
       <c r="O12" t="str">
-        <f t="shared" ca="1" si="1"/>
         <v>Carrot</v>
       </c>
-      <c r="P12" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Lobster</v>
-      </c>
-      <c r="Q12" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Pasta</v>
-      </c>
-      <c r="R12" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Bread</v>
-      </c>
-      <c r="S12" t="str" cm="1">
-        <f t="array" aca="1" ref="S12" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Chicken</v>
-      </c>
-      <c r="U12">
-        <f ca="1">COUNTIF($K$12:$S$12,U6)</f>
-        <v>1</v>
-      </c>
-      <c r="V12">
-        <f ca="1">MAX(0,COUNTIF($K$12:$S$12,V6)-(U6=V6))</f>
-        <v>1</v>
-      </c>
-      <c r="W12">
-        <f ca="1">MAX(0, COUNTIF($K$12:$S$12,W6)-(W6=V6)-(W6=U6))</f>
-        <v>0</v>
-      </c>
-      <c r="X12">
-        <f ca="1">SUM(U12:W12)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="2:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D13">
         <v>10</v>
       </c>
       <c r="E13">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="F13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="O13" t="str">
+        <v>Onion</v>
+      </c>
+    </row>
+    <row r="14" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
@@ -1267,15 +1044,18 @@
         <v>10</v>
       </c>
       <c r="E14">
-        <v>25</v>
+        <v>95</v>
       </c>
       <c r="F14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="O14" t="str">
+        <v>Lettuce</v>
+      </c>
+    </row>
+    <row r="15" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
@@ -1284,131 +1064,178 @@
         <v>10</v>
       </c>
       <c r="E15">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="F15">
         <v>1</v>
       </c>
-      <c r="U15" t="str">
-        <f ca="1">INDEX(Food[Name],RANDBETWEEN(0,COUNTA(_xlfn.ANCHORARRAY(U17))))</f>
+    </row>
+    <row r="16" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16">
+        <v>10</v>
+      </c>
+      <c r="E16">
+        <v>15</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="L16" t="str" cm="1">
+        <f t="array" ref="L16:L24">_xlfn._xlws.FILTER(Food[Name],COUNTIF(AA3:AC3, Food[Type])&gt;0,"-")</f>
+        <v>Bread</v>
+      </c>
+    </row>
+    <row r="17" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="L17" t="str">
+        <v>Pasta</v>
+      </c>
+    </row>
+    <row r="18" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="L18" t="str">
+        <v>Rice</v>
+      </c>
+    </row>
+    <row r="19" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="L19" t="str">
+        <v>Beef</v>
+      </c>
+    </row>
+    <row r="20" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="L20" t="str">
+        <v>Pork</v>
+      </c>
+    </row>
+    <row r="21" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="L21" t="str">
+        <v>Chicken</v>
+      </c>
+    </row>
+    <row r="22" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="F22" t="e">
+        <f ca="1">INDEX(Food[Name],RANDBETWEEN(0,COUNTA(_xlfn.ANCHORARRAY(L17))))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G22" t="e" cm="1">
+        <f t="array" aca="1" ref="G22" ca="1">_xlfn.SINGLE(INDEX(_xlfn._xlws.FILTER(Food[],Food[Points] = OR(OrderIncludes,OrderIncludes2,OrderIncludes3), "ERR"),RANDBETWEEN(0,3)))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I22" t="e" cm="1">
+        <f t="array" aca="1" ref="I22" ca="1">_xlfn.SINGLE(INDEX(_xlfn._xlws.FILTER(Food[],Food[Type] =NOT(OrderIncludes), "ERR"),RANDBETWEEN(0,3)))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L22" t="str">
+        <v>Carrot</v>
+      </c>
+    </row>
+    <row r="23" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="G23" t="str" cm="1">
+        <f t="array" aca="1" ref="G23" ca="1">INDEX(_xlfn.ANCHORARRAY(AvailableItems), RANDBETWEEN(1, ROWS(_xlfn.ANCHORARRAY(AvailableItems))))</f>
+        <v>Carrot</v>
+      </c>
+      <c r="L23" t="str">
+        <v>Onion</v>
+      </c>
+    </row>
+    <row r="24" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="L24" t="str">
         <v>Lettuce</v>
       </c>
-      <c r="V15" t="e" cm="1">
-        <f t="array" aca="1" ref="V15" ca="1">_xlfn.SINGLE(INDEX(_xlfn._xlws.FILTER(Food[],Food[Points] = OR(OrderIncludes,OrderIncludes2,OrderIncludes3), "ERR"),RANDBETWEEN(0,3)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="W15" t="e" cm="1">
-        <f t="array" aca="1" ref="W15" ca="1">_xlfn.SINGLE(INDEX(_xlfn._xlws.FILTER(Food[],Food[Type] =NOT(OrderIncludes), "ERR"),RANDBETWEEN(0,3)))</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="16" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="U16" t="str" cm="1">
-        <f t="array" ref="U16:U24">_xlfn._xlws.FILTER(Food[Name],COUNTIF(U2:W2, Food[Type])&gt;0,"-")</f>
+    </row>
+    <row r="29" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E30">
+        <f ca="1">RANDBETWEEN(1,COUNTA(_xlfn.ANCHORARRAY(AvailableItems)))</f>
+        <v>3</v>
+      </c>
+      <c r="F30">
+        <f ca="1">RANDBETWEEN(1,COUNTA(_xlfn.ANCHORARRAY(AvailableItems)))</f>
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <f ca="1">RANDBETWEEN(1,COUNTA(_xlfn.ANCHORARRAY(AvailableItems)))</f>
+        <v>5</v>
+      </c>
+      <c r="K30" t="str" cm="1">
+        <f t="array" aca="1" ref="K30" ca="1">IF(INDEX(Food[Name],OrderIndex2)= OR(OrderIndex,OrderIndex3), "-",INDEX(Food[Name],OrderIndex2))</f>
+        <v>Salmon</v>
+      </c>
+    </row>
+    <row r="31" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E31">
+        <f ca="1">RANDBETWEEN(1,COUNTA(_xlfn.ANCHORARRAY(AvailableItems)))</f>
+        <v>6</v>
+      </c>
+      <c r="F31">
+        <f ca="1">RANDBETWEEN(1,COUNTA(_xlfn.ANCHORARRAY(AvailableItems)))</f>
+        <v>6</v>
+      </c>
+      <c r="G31">
+        <f ca="1">RANDBETWEEN(1,COUNTA(_xlfn.ANCHORARRAY(AvailableItems)))</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E32">
+        <f ca="1">RANDBETWEEN(1,COUNTA(_xlfn.ANCHORARRAY(AvailableItems)))</f>
+        <v>2</v>
+      </c>
+      <c r="F32">
+        <f ca="1">RANDBETWEEN(1,COUNTA(_xlfn.ANCHORARRAY(AvailableItems)))</f>
+        <v>6</v>
+      </c>
+      <c r="G32">
+        <f ca="1">RANDBETWEEN(1,COUNTA(_xlfn.ANCHORARRAY(AvailableItems)))</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G37" t="str" cm="1">
+        <f t="array" ref="G37:H39">_xlfn._xlws.FILTER(Food[[Name]:[Type]],Food[Type]=OrderIncludes,"-")</f>
         <v>Bread</v>
       </c>
-      <c r="V16" t="str" cm="1">
-        <f t="array" aca="1" ref="V16" ca="1">INDEX(_xlfn.ANCHORARRAY(U16), RANDBETWEEN(1, ROWS(_xlfn.ANCHORARRAY(U16))))</f>
+      <c r="H37" t="str">
+        <v>Grain</v>
+      </c>
+    </row>
+    <row r="38" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G38" t="str">
         <v>Pasta</v>
       </c>
-    </row>
-    <row r="17" spans="9:23" x14ac:dyDescent="0.25">
-      <c r="U17" t="str">
-        <v>Pasta</v>
-      </c>
-    </row>
-    <row r="18" spans="9:23" x14ac:dyDescent="0.25">
-      <c r="U18" t="str">
+      <c r="H38" t="str">
+        <v>Grain</v>
+      </c>
+    </row>
+    <row r="39" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G39" t="str">
         <v>Rice</v>
       </c>
-    </row>
-    <row r="19" spans="9:23" x14ac:dyDescent="0.25">
-      <c r="I19" t="s">
-        <v>31</v>
-      </c>
-      <c r="U19" t="str">
-        <v>Beef</v>
-      </c>
-    </row>
-    <row r="20" spans="9:23" x14ac:dyDescent="0.25">
-      <c r="U20" t="str">
-        <v>Pork</v>
-      </c>
-    </row>
-    <row r="21" spans="9:23" x14ac:dyDescent="0.25">
-      <c r="N21" t="s">
-        <v>30</v>
-      </c>
-      <c r="U21" t="str">
-        <v>Chicken</v>
-      </c>
-    </row>
-    <row r="22" spans="9:23" x14ac:dyDescent="0.25">
-      <c r="N22">
-        <f ca="1">RANDBETWEEN(1,COUNTA(Food[Name]))</f>
-        <v>8</v>
-      </c>
-      <c r="O22">
-        <f ca="1">RANDBETWEEN(1,COUNTA(Food[Type]))</f>
-        <v>6</v>
-      </c>
-      <c r="P22">
-        <f ca="1">RANDBETWEEN(1,COUNTA(Food[Points]))</f>
-        <v>9</v>
-      </c>
-      <c r="R22" t="str" cm="1">
-        <f t="array" aca="1" ref="R22" ca="1">IF(INDEX(Food[Name],OrderIndex2)= OR(OrderIndex,OrderIndex3), "-",INDEX(Food[Name],OrderIndex2))</f>
-        <v>Rice</v>
-      </c>
-      <c r="U22" t="str">
-        <v>Carrot</v>
-      </c>
-    </row>
-    <row r="23" spans="9:23" x14ac:dyDescent="0.25">
-      <c r="U23" t="str">
-        <v>Onion</v>
-      </c>
-    </row>
-    <row r="24" spans="9:23" x14ac:dyDescent="0.25">
-      <c r="U24" t="str">
-        <v>Lettuce</v>
-      </c>
-    </row>
-    <row r="30" spans="9:23" x14ac:dyDescent="0.25">
-      <c r="V30" t="str" cm="1">
-        <f t="array" ref="V30:W32">_xlfn._xlws.FILTER(Food[[Name]:[Type]],Food[Type]=OrderIncludes,"-")</f>
-        <v>Bread</v>
-      </c>
-      <c r="W30" t="str">
+      <c r="H39" t="str">
         <v>Grain</v>
       </c>
     </row>
-    <row r="31" spans="9:23" x14ac:dyDescent="0.25">
-      <c r="V31" t="str">
-        <v>Pasta</v>
-      </c>
-      <c r="W31" t="str">
-        <v>Grain</v>
-      </c>
-    </row>
-    <row r="32" spans="9:23" x14ac:dyDescent="0.25">
-      <c r="V32" t="str">
-        <v>Rice</v>
-      </c>
-      <c r="W32" t="str">
-        <v>Grain</v>
-      </c>
-    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="L4:N4"/>
+  </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C15 U2:W2" xr:uid="{22784EBF-D91C-4A9F-BBF6-DF997D832606}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C16 AA3:AC3 L5:N5" xr:uid="{22784EBF-D91C-4A9F-BBF6-DF997D832606}">
       <formula1>INDIRECT("ItemTypes[Type]")</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F15" xr:uid="{974DD810-82B8-4D7E-B93F-00E192FD871B}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F16" xr:uid="{974DD810-82B8-4D7E-B93F-00E192FD871B}">
       <formula1>1</formula1>
       <formula2>2</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4:E15" xr:uid="{F145B394-3EE5-45DA-BD07-F9070E8EDA1D}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E16" xr:uid="{F145B394-3EE5-45DA-BD07-F9070E8EDA1D}">
       <formula1>1</formula1>
       <formula2>100</formula2>
     </dataValidation>
@@ -1421,24 +1248,21 @@
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="97dd5345-e793-494f-a61a-0ff5f2d8588d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C394FD4D-B2A9-4197-A8FB-06556B04AB33}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:Q22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EB9F34A24037AB4FA470085E68A4B53B" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1f05ce8c82e9282909648c3323760eae">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="97dd5345-e793-494f-a61a-0ff5f2d8588d" xmlns:ns4="72e2bb9d-dac6-4618-b85f-5ec835598a0c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c14bf05b446930f087596548c801372f" ns3:_="" ns4:_="">
     <xsd:import namespace="97dd5345-e793-494f-a61a-0ff5f2d8588d"/>
@@ -1665,32 +1489,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA6B1F78-6D1D-4550-867C-D81A2584596E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="72e2bb9d-dac6-4618-b85f-5ec835598a0c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="97dd5345-e793-494f-a61a-0ff5f2d8588d"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB2BC082-80AE-42F8-9667-95CF6F1F5700}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="97dd5345-e793-494f-a61a-0ff5f2d8588d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{65537B17-CCB8-447E-A12B-556BEEDE4DB0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1707,4 +1523,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB2BC082-80AE-42F8-9667-95CF6F1F5700}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA6B1F78-6D1D-4550-867C-D81A2584596E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="72e2bb9d-dac6-4618-b85f-5ec835598a0c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="97dd5345-e793-494f-a61a-0ff5f2d8588d"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added some conditional formatting so Its more readable
Still dont properly understand how i could use or but who really cares
</commit_message>
<xml_diff>
--- a/UntitledKitchenGame/Game/UntitledKitchenGame/Assets/Editor/Items.xlsx
+++ b/UntitledKitchenGame/Game/UntitledKitchenGame/Assets/Editor/Items.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\murra\OneDrive\Documents\GitHub\UntitledKitchenGame\UntitledKitchenGame\Game\UntitledKitchenGame\Assets\Editor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF09E6A1-EC52-4582-B53A-66D846B25D84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{248452DA-9A49-42ED-ADAC-0B8CB9CCF070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F8B15126-9F65-4AA0-BFBE-7FC0EBE8032D}"/>
   </bookViews>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="34">
   <si>
     <t>Points</t>
   </si>
@@ -112,9 +112,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Order</t>
-  </si>
-  <si>
     <t>Item 1</t>
   </si>
   <si>
@@ -148,7 +145,7 @@
     <t>Lettuce</t>
   </si>
   <si>
-    <t>New Item</t>
+    <t>Items</t>
   </si>
   <si>
     <t>Order Includes…</t>
@@ -167,13 +164,22 @@
   </si>
   <si>
     <t>AvailableItems</t>
+  </si>
+  <si>
+    <t>Order 1 Possible</t>
+  </si>
+  <si>
+    <t>Order 2 Possible</t>
+  </si>
+  <si>
+    <t>Order 3 Possible</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -189,27 +195,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="2"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -254,25 +246,299 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="41">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -293,7 +559,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{35FB6A7E-F941-41ED-AF7A-CE78317F833A}" name="ItemTypes" displayName="ItemTypes" ref="H4:H8" totalsRowShown="0" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{35FB6A7E-F941-41ED-AF7A-CE78317F833A}" name="ItemTypes" displayName="ItemTypes" ref="H4:H8" totalsRowShown="0" headerRowDxfId="40">
   <autoFilter ref="H4:H8" xr:uid="{35FB6A7E-F941-41ED-AF7A-CE78317F833A}">
     <filterColumn colId="0" hiddenButton="1"/>
   </autoFilter>
@@ -305,7 +571,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7AE9A713-C3CE-48AC-B440-488A7CD3381A}" name="Food" displayName="Food" ref="B4:F16" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7AE9A713-C3CE-48AC-B440-488A7CD3381A}" name="Food" displayName="Food" ref="B4:F16" totalsRowShown="0" headerRowDxfId="39">
   <autoFilter ref="B4:F16" xr:uid="{7AE9A713-C3CE-48AC-B440-488A7CD3381A}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:F16">
     <sortCondition ref="C4:C16"/>
@@ -638,10 +904,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2334730F-D581-4249-91BD-F969B819BCBB}">
-  <dimension ref="B2:AI39"/>
+  <dimension ref="B2:AL39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="AE19" sqref="AE19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -651,41 +917,44 @@
     <col min="11" max="11" width="11.7109375" customWidth="1"/>
     <col min="12" max="24" width="9.42578125" customWidth="1"/>
     <col min="30" max="30" width="9.7109375" customWidth="1"/>
+    <col min="36" max="36" width="16.28515625" customWidth="1"/>
+    <col min="37" max="37" width="15.85546875" customWidth="1"/>
+    <col min="38" max="38" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="AA2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB2" s="2"/>
-      <c r="AC2" s="2"/>
+    <row r="2" spans="2:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AA2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB2" s="5"/>
+      <c r="AC2" s="5"/>
       <c r="AD2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG2" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="AG2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="AH2" s="2"/>
-      <c r="AI2" s="2"/>
-    </row>
-    <row r="3" spans="2:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Y3" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA3" s="4" t="s">
+      <c r="AH2" s="5"/>
+      <c r="AI2" s="5"/>
+    </row>
+    <row r="3" spans="2:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q3" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="AB3" s="4" t="s">
+      <c r="AB3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="AC3" s="4" t="s">
+      <c r="AC3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="AG3" s="2"/>
-      <c r="AH3" s="2"/>
-      <c r="AI3" s="2"/>
-    </row>
-    <row r="4" spans="2:35" s="1" customFormat="1" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AG3" s="5"/>
+      <c r="AH3" s="5"/>
+      <c r="AI3" s="5"/>
+    </row>
+    <row r="4" spans="2:38" s="1" customFormat="1" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>12</v>
       </c>
@@ -705,45 +974,51 @@
         <v>1</v>
       </c>
       <c r="K4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="AA4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AI4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AJ4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="Z4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="AB4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="AC4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="AD4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="AE4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="AF4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AG4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="AH4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="AI4" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="2:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AK4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AL4" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="2:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>9</v>
       </c>
@@ -762,94 +1037,106 @@
       <c r="H5" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="6">
+      <c r="K5" s="4">
         <v>3</v>
       </c>
-      <c r="L5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="M5" s="4" t="s">
+      <c r="L5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="N5" s="4" t="s">
+      <c r="M5" s="2" t="s">
         <v>5</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="Q5" t="str" cm="1">
         <f t="array" aca="1" ref="Q5" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Pork</v>
+        <v>Beef</v>
       </c>
       <c r="R5" t="str" cm="1">
         <f t="array" aca="1" ref="R5" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Pork</v>
+        <v>Carrot</v>
       </c>
       <c r="S5" t="str" cm="1">
         <f t="array" aca="1" ref="S5" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Salmon</v>
+        <v>Carrot</v>
       </c>
       <c r="T5" t="str" cm="1">
         <f t="array" aca="1" ref="T5" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Carrot</v>
+        <v>Lettuce</v>
       </c>
       <c r="U5" t="str" cm="1">
         <f t="array" aca="1" ref="U5" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Pasta</v>
+        <v>Lobster</v>
       </c>
       <c r="V5" t="str" cm="1">
         <f t="array" aca="1" ref="V5" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Salmon</v>
+        <v>Carrot</v>
       </c>
       <c r="W5" t="str" cm="1">
         <f t="array" aca="1" ref="W5" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Lettuce</v>
+        <v>Beef</v>
       </c>
       <c r="X5" t="str" cm="1">
         <f t="array" aca="1" ref="X5" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Onion</v>
+        <v>Pasta</v>
       </c>
       <c r="Y5" t="str" cm="1">
         <f t="array" aca="1" ref="Y5" ca="1">INDEX(Food[Name],RANDBETWEEN(1,COUNTA(Food[Name])))</f>
-        <v>Salmon</v>
-      </c>
-      <c r="AA5" s="2" t="str" cm="1">
+        <v>Lobster</v>
+      </c>
+      <c r="AA5" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="AA5" ca="1">IF(INDEX(_xlfn.ANCHORARRAY(AvailableItems),OrderIndex)= OR(OrderIndex2,OrderIndex3),"FirstConTrue", INDEX(_xlfn.ANCHORARRAY(AvailableItems),OrderIndex))</f>
-        <v>Rice</v>
-      </c>
-      <c r="AB5" s="2" t="str" cm="1">
+        <v>Pasta</v>
+      </c>
+      <c r="AB5" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="AB5" ca="1">IF(INDEX(_xlfn.ANCHORARRAY(AvailableItems),OrderIndex2)= OR(OrderIndex,OrderIndex3),"FirstConTrue", INDEX(_xlfn.ANCHORARRAY(AvailableItems),OrderIndex2))</f>
-        <v>Bread</v>
-      </c>
-      <c r="AC5" s="2" t="str" cm="1">
+        <v>Beef</v>
+      </c>
+      <c r="AC5" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="AC5" ca="1">IF(INDEX(_xlfn.ANCHORARRAY(AvailableItems),OrderIndex3)= OR(OrderIndex2,OrderIndex),"FirstConTrue", INDEX(_xlfn.ANCHORARRAY(AvailableItems),OrderIndex3))</f>
-        <v>Pork</v>
+        <v>Pasta</v>
       </c>
       <c r="AD5" t="str" cm="1">
         <f t="array" aca="1" ref="AD5" ca="1">IF(INDEX(_xlfn.ANCHORARRAY(AvailableItems),E31)= OR(F31,G31),"FirstConTrue", INDEX(_xlfn.ANCHORARRAY(AvailableItems),E31))</f>
-        <v>Chicken</v>
+        <v>Pork</v>
       </c>
       <c r="AE5" t="str" cm="1">
         <f t="array" aca="1" ref="AE5" ca="1">IF(INDEX(_xlfn.ANCHORARRAY(AvailableItems),F31)= OR(G31,E31),"FirstConTrue", INDEX(_xlfn.ANCHORARRAY(AvailableItems),F31))</f>
-        <v>Chicken</v>
+        <v>Rice</v>
       </c>
       <c r="AF5" t="str" cm="1">
         <f t="array" aca="1" ref="AF5" ca="1">IF(INDEX(_xlfn.ANCHORARRAY(AvailableItems),G31)= OR(E31,F31),"FirstConTrue", INDEX(_xlfn.ANCHORARRAY(AvailableItems),G31))</f>
+        <v>Rice</v>
+      </c>
+      <c r="AG5" s="5" t="str" cm="1">
+        <f t="array" aca="1" ref="AG5" ca="1">IF(INDEX(_xlfn.ANCHORARRAY(AvailableItems),E32)= OR(F32,G32),"FirstConTrue", INDEX(_xlfn.ANCHORARRAY(AvailableItems),E32))</f>
         <v>Chicken</v>
       </c>
-      <c r="AG5" s="2" t="str" cm="1">
-        <f t="array" aca="1" ref="AG5" ca="1">IF(INDEX(_xlfn.ANCHORARRAY(AvailableItems),E32)= OR(F32,G32),"FirstConTrue", INDEX(_xlfn.ANCHORARRAY(AvailableItems),E32))</f>
-        <v>Pasta</v>
-      </c>
-      <c r="AH5" s="2" t="str" cm="1">
+      <c r="AH5" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="AH5" ca="1">IF(INDEX(_xlfn.ANCHORARRAY(AvailableItems),F32)= OR(G32,E32),"FirstConTrue", INDEX(_xlfn.ANCHORARRAY(AvailableItems),F32))</f>
-        <v>Chicken</v>
-      </c>
-      <c r="AI5" s="2" t="str" cm="1">
+        <v>Pork</v>
+      </c>
+      <c r="AI5" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="AI5" ca="1">IF(INDEX(_xlfn.ANCHORARRAY(AvailableItems),G32)= OR(F32,E32),"FirstConTrue", INDEX(_xlfn.ANCHORARRAY(AvailableItems),G32))</f>
-        <v>Rice</v>
-      </c>
-    </row>
-    <row r="6" spans="2:35" x14ac:dyDescent="0.25">
+        <v>Carrot</v>
+      </c>
+      <c r="AJ5" t="b">
+        <f ca="1">IF(COUNTIF($Q5:$Y5,AA5)+COUNTIF($Q5:$Y5,AB5)+COUNTIF($Q5:$Y5,AC5)&gt;=3,TRUE, FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="AK5" t="b">
+        <f ca="1">IF(COUNTIF($Q5:$Y5,AF5)+COUNTIF($Q5:$Y5,AE5)+COUNTIF($Q5:$Y5,AD5)&gt;=3,TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AL5" t="b">
+        <f ca="1">IF(COUNTIF($Q5:$Y5,AI5)+COUNTIF($Q5:$Y5,AH5)+COUNTIF($Q5:$Y5,AG5)&gt;=3,TRUE, FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -872,12 +1159,12 @@
       <c r="N6" s="1"/>
       <c r="O6" s="1" t="str" cm="1">
         <f t="array" ref="O6:O14">_xlfn._xlws.FILTER(Food[Name],COUNTIF(L5:N5, Food[Type])&gt;0,"-")</f>
-        <v>Bread</v>
-      </c>
-    </row>
-    <row r="7" spans="2:35" x14ac:dyDescent="0.25">
+        <v>Salmon</v>
+      </c>
+    </row>
+    <row r="7" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
@@ -895,18 +1182,18 @@
         <v>6</v>
       </c>
       <c r="K7">
-        <f>_xlfn.BINOM.DIST(OrderMax,COUNTA(_xlfn.ANCHORARRAY(O6)),1/COUNTA(_xlfn.ANCHORARRAY(O6)),TRUE)</f>
-        <v>0.98789364751434194</v>
+        <f>_xlfn.BINOM.DIST(OrderMax,COUNTA(_xlfn.ANCHORARRAY(O6)),1/COUNTA(_xlfn.ANCHORARRAY(O6)),)</f>
+        <v>5.6837716706304615E-2</v>
       </c>
       <c r="O7" t="str">
-        <v>Pasta</v>
+        <v>Tuna</v>
       </c>
       <c r="AD7" t="str">
         <f t="shared" ref="AD7" si="0">_xlfn.CONCAT(P7:Y7)</f>
         <v/>
       </c>
     </row>
-    <row r="8" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>11</v>
       </c>
@@ -926,16 +1213,16 @@
         <v>10</v>
       </c>
       <c r="O8" t="str">
-        <v>Rice</v>
+        <v>Lobster</v>
       </c>
       <c r="AD8" t="str">
         <f>_xlfn.CONCAT(P8:Y8)</f>
         <v/>
       </c>
     </row>
-    <row r="9" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
@@ -953,9 +1240,9 @@
         <v>Beef</v>
       </c>
     </row>
-    <row r="10" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
         <v>10</v>
@@ -973,7 +1260,7 @@
         <v>Pork</v>
       </c>
     </row>
-    <row r="11" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>7</v>
       </c>
@@ -993,9 +1280,9 @@
         <v>Chicken</v>
       </c>
     </row>
-    <row r="12" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
@@ -1013,9 +1300,9 @@
         <v>Carrot</v>
       </c>
     </row>
-    <row r="13" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -1033,7 +1320,7 @@
         <v>Onion</v>
       </c>
     </row>
-    <row r="14" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>8</v>
       </c>
@@ -1053,9 +1340,9 @@
         <v>Lettuce</v>
       </c>
     </row>
-    <row r="15" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
@@ -1070,9 +1357,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C16" t="s">
         <v>5</v>
@@ -1117,9 +1404,9 @@
       </c>
     </row>
     <row r="22" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="F22" t="e">
+      <c r="F22" t="str">
         <f ca="1">INDEX(Food[Name],RANDBETWEEN(0,COUNTA(_xlfn.ANCHORARRAY(L17))))</f>
-        <v>#VALUE!</v>
+        <v>Salmon</v>
       </c>
       <c r="G22" t="e" cm="1">
         <f t="array" aca="1" ref="G22" ca="1">_xlfn.SINGLE(INDEX(_xlfn._xlws.FILTER(Food[],Food[Points] = OR(OrderIncludes,OrderIncludes2,OrderIncludes3), "ERR"),RANDBETWEEN(0,3)))</f>
@@ -1136,7 +1423,7 @@
     <row r="23" spans="5:12" x14ac:dyDescent="0.25">
       <c r="G23" t="str" cm="1">
         <f t="array" aca="1" ref="G23" ca="1">INDEX(_xlfn.ANCHORARRAY(AvailableItems), RANDBETWEEN(1, ROWS(_xlfn.ANCHORARRAY(AvailableItems))))</f>
-        <v>Carrot</v>
+        <v>Rice</v>
       </c>
       <c r="L23" t="str">
         <v>Onion</v>
@@ -1149,53 +1436,53 @@
     </row>
     <row r="29" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E30">
         <f ca="1">RANDBETWEEN(1,COUNTA(_xlfn.ANCHORARRAY(AvailableItems)))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F30">
         <f ca="1">RANDBETWEEN(1,COUNTA(_xlfn.ANCHORARRAY(AvailableItems)))</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G30">
         <f ca="1">RANDBETWEEN(1,COUNTA(_xlfn.ANCHORARRAY(AvailableItems)))</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K30" t="str" cm="1">
         <f t="array" aca="1" ref="K30" ca="1">IF(INDEX(Food[Name],OrderIndex2)= OR(OrderIndex,OrderIndex3), "-",INDEX(Food[Name],OrderIndex2))</f>
-        <v>Salmon</v>
+        <v>Bread</v>
       </c>
     </row>
     <row r="31" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E31">
         <f ca="1">RANDBETWEEN(1,COUNTA(_xlfn.ANCHORARRAY(AvailableItems)))</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F31">
         <f ca="1">RANDBETWEEN(1,COUNTA(_xlfn.ANCHORARRAY(AvailableItems)))</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G31">
         <f ca="1">RANDBETWEEN(1,COUNTA(_xlfn.ANCHORARRAY(AvailableItems)))</f>
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E32">
         <f ca="1">RANDBETWEEN(1,COUNTA(_xlfn.ANCHORARRAY(AvailableItems)))</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F32">
         <f ca="1">RANDBETWEEN(1,COUNTA(_xlfn.ANCHORARRAY(AvailableItems)))</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G32">
         <f ca="1">RANDBETWEEN(1,COUNTA(_xlfn.ANCHORARRAY(AvailableItems)))</f>
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="37" spans="7:8" x14ac:dyDescent="0.25">
@@ -1245,6 +1532,125 @@
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="10" operator="containsText" id="{6CF41F10-0181-49CA-AA67-062D7C58386F}">
+            <xm:f>NOT(ISERROR(SEARCH($AA$5,Q5)))</xm:f>
+            <xm:f>$AA$5</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="9"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="9" operator="containsText" id="{434E2E08-0F2B-421B-B0FB-62E7CFF6D678}">
+            <xm:f>NOT(ISERROR(SEARCH($AB$5,Q5)))</xm:f>
+            <xm:f>$AB$5</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="9"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="8" operator="containsText" id="{0507535D-E0F8-4081-A7DB-D7CDC562C502}">
+            <xm:f>NOT(ISERROR(SEARCH($AC$5,Q5)))</xm:f>
+            <xm:f>$AC$5</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="9"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="7" operator="containsText" id="{BA02B6FE-085F-4B16-8DA8-D48894BEDF08}">
+            <xm:f>NOT(ISERROR(SEARCH(OR($AD$5,$AE$5,$AF$5),Q5)))</xm:f>
+            <xm:f>OR($AD$5,$AE$5,$AF$5)</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="4"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="6" operator="containsText" id="{6E30C0C3-B60E-41DC-A3FF-6237DECB771A}">
+            <xm:f>NOT(ISERROR(SEARCH($AD$5,Q5)))</xm:f>
+            <xm:f>$AD$5</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="4"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="5" operator="containsText" id="{ED8773FC-9691-4256-88FE-D8CA21D43B55}">
+            <xm:f>NOT(ISERROR(SEARCH($AE$5,Q5)))</xm:f>
+            <xm:f>$AE$5</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="4"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="4" operator="containsText" id="{BDB8547B-5883-4046-8378-AF69BFD8C777}">
+            <xm:f>NOT(ISERROR(SEARCH($AF$5,Q5)))</xm:f>
+            <xm:f>$AF$5</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="4"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="3" operator="containsText" id="{2A2BCC8F-5518-4C00-97FA-8E8D48DE6C30}">
+            <xm:f>NOT(ISERROR(SEARCH($AG$5,Q5)))</xm:f>
+            <xm:f>$AG$5</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="5"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="2" operator="containsText" id="{F40545B5-4F29-4283-8AC0-ED0AE2970D69}">
+            <xm:f>NOT(ISERROR(SEARCH($AH$5,Q5)))</xm:f>
+            <xm:f>$AH$5</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="5"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{8410C135-9AFC-4284-9432-34FF6120BC75}">
+            <xm:f>NOT(ISERROR(SEARCH($AI$5,Q5)))</xm:f>
+            <xm:f>$AI$5</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="5"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>Q5:Y5</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 

</xml_diff>